<commit_message>
changed date 14 sleep
</commit_message>
<xml_diff>
--- a/viki.xlsx
+++ b/viki.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikib\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikib\Desktop\PROGRAMS\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4532BF-D22C-467B-9DEA-7038C4D3B0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0226C8-E0E2-400E-9A2D-E1BF05560317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="599" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly" sheetId="1" r:id="rId1"/>
@@ -2315,6 +2315,36 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2336,37 +2366,22 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2396,21 +2411,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2426,19 +2426,96 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2448,46 +2525,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2499,8 +2561,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2525,97 +2594,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2628,9 +2631,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2985,8 +2985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AE239"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E230" sqref="E230"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G230" sqref="G230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3723,13 +3723,13 @@
       <c r="W21" s="10"/>
     </row>
     <row r="22" spans="3:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="323">
+      <c r="F22" s="311">
         <f>SUM(F21:I21)</f>
         <v>3.4090277777777782</v>
       </c>
-      <c r="G22" s="324"/>
-      <c r="H22" s="324"/>
-      <c r="I22" s="325"/>
+      <c r="G22" s="312"/>
+      <c r="H22" s="312"/>
+      <c r="I22" s="313"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
@@ -4903,16 +4903,16 @@
       </c>
     </row>
     <row r="61" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="F61" s="321">
+      <c r="F61" s="320">
         <f>SUM(F60:L60)</f>
         <v>4.1243055555555559</v>
       </c>
-      <c r="G61" s="321"/>
-      <c r="H61" s="321"/>
-      <c r="I61" s="321"/>
-      <c r="J61" s="321"/>
-      <c r="K61" s="321"/>
-      <c r="L61" s="321"/>
+      <c r="G61" s="320"/>
+      <c r="H61" s="320"/>
+      <c r="I61" s="320"/>
+      <c r="J61" s="320"/>
+      <c r="K61" s="320"/>
+      <c r="L61" s="320"/>
       <c r="O61" s="36"/>
     </row>
     <row r="63" spans="3:18" x14ac:dyDescent="0.3">
@@ -4999,7 +4999,7 @@
       </c>
       <c r="P65" s="34"/>
       <c r="Q65" s="63"/>
-      <c r="R65" s="326">
+      <c r="R65" s="317">
         <f>SUM(N65:N71)</f>
         <v>1.0555555555555556</v>
       </c>
@@ -5035,7 +5035,7 @@
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="64"/>
-      <c r="R66" s="327"/>
+      <c r="R66" s="318"/>
     </row>
     <row r="67" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C67" s="4">
@@ -5076,7 +5076,7 @@
       <c r="Q67" s="64">
         <v>1</v>
       </c>
-      <c r="R67" s="327"/>
+      <c r="R67" s="318"/>
     </row>
     <row r="68" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C68" s="4">
@@ -5113,7 +5113,7 @@
       <c r="Q68" s="64">
         <v>1</v>
       </c>
-      <c r="R68" s="327"/>
+      <c r="R68" s="318"/>
     </row>
     <row r="69" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C69" s="4">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="P69" s="4"/>
       <c r="Q69" s="64"/>
-      <c r="R69" s="327"/>
+      <c r="R69" s="318"/>
     </row>
     <row r="70" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C70" s="4">
@@ -5191,7 +5191,7 @@
       </c>
       <c r="P70" s="4"/>
       <c r="Q70" s="64"/>
-      <c r="R70" s="327"/>
+      <c r="R70" s="318"/>
     </row>
     <row r="71" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C71" s="66">
@@ -5228,7 +5228,7 @@
       <c r="Q71" s="69">
         <v>1</v>
       </c>
-      <c r="R71" s="328"/>
+      <c r="R71" s="319"/>
     </row>
     <row r="72" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C72" s="4">
@@ -5267,7 +5267,7 @@
       <c r="Q72" s="64">
         <v>1</v>
       </c>
-      <c r="R72" s="326">
+      <c r="R72" s="317">
         <f>SUM(N72:N78)</f>
         <v>1.2590277777777779</v>
       </c>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="P73" s="4"/>
       <c r="Q73" s="64"/>
-      <c r="R73" s="327"/>
+      <c r="R73" s="318"/>
     </row>
     <row r="74" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C74" s="4">
@@ -5350,7 +5350,7 @@
       <c r="Q74" s="64">
         <v>1</v>
       </c>
-      <c r="R74" s="327"/>
+      <c r="R74" s="318"/>
     </row>
     <row r="75" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C75" s="4">
@@ -5385,7 +5385,7 @@
       <c r="Q75" s="64">
         <v>1</v>
       </c>
-      <c r="R75" s="327"/>
+      <c r="R75" s="318"/>
     </row>
     <row r="76" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C76" s="4">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="P76" s="4"/>
       <c r="Q76" s="64"/>
-      <c r="R76" s="327"/>
+      <c r="R76" s="318"/>
     </row>
     <row r="77" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C77" s="4">
@@ -5461,7 +5461,7 @@
       <c r="Q77" s="64">
         <v>1</v>
       </c>
-      <c r="R77" s="327"/>
+      <c r="R77" s="318"/>
     </row>
     <row r="78" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C78" s="66">
@@ -5500,7 +5500,7 @@
       <c r="Q78" s="69">
         <v>1</v>
       </c>
-      <c r="R78" s="328"/>
+      <c r="R78" s="319"/>
     </row>
     <row r="79" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C79" s="4">
@@ -5535,7 +5535,7 @@
         <v>0.24861111111111112</v>
       </c>
       <c r="Q79" s="64"/>
-      <c r="R79" s="326">
+      <c r="R79" s="317">
         <f>SUM(N79:N85)</f>
         <v>1.3118055555555554</v>
       </c>
@@ -5579,7 +5579,7 @@
       <c r="Q80" s="64">
         <v>1</v>
       </c>
-      <c r="R80" s="327"/>
+      <c r="R80" s="318"/>
     </row>
     <row r="81" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C81" s="4">
@@ -5620,7 +5620,7 @@
         <v>1.5277777777777777E-2</v>
       </c>
       <c r="Q81" s="64"/>
-      <c r="R81" s="327"/>
+      <c r="R81" s="318"/>
     </row>
     <row r="82" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C82" s="4">
@@ -5663,7 +5663,7 @@
       <c r="Q82" s="64">
         <v>1</v>
       </c>
-      <c r="R82" s="327"/>
+      <c r="R82" s="318"/>
     </row>
     <row r="83" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C83" s="4">
@@ -5702,7 +5702,7 @@
       </c>
       <c r="P83" s="4"/>
       <c r="Q83" s="64"/>
-      <c r="R83" s="327"/>
+      <c r="R83" s="318"/>
     </row>
     <row r="84" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C84" s="4">
@@ -5745,7 +5745,7 @@
       <c r="Q84" s="64">
         <v>1</v>
       </c>
-      <c r="R84" s="327"/>
+      <c r="R84" s="318"/>
     </row>
     <row r="85" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C85" s="66">
@@ -5780,7 +5780,7 @@
       </c>
       <c r="P85" s="66"/>
       <c r="Q85" s="69"/>
-      <c r="R85" s="328"/>
+      <c r="R85" s="319"/>
     </row>
     <row r="86" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C86" s="4">
@@ -6176,16 +6176,16 @@
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
       <c r="E96" s="10"/>
-      <c r="F96" s="318">
+      <c r="F96" s="314">
         <f>SUM(F95:L95)</f>
         <v>5.4020833333333336</v>
       </c>
-      <c r="G96" s="319"/>
-      <c r="H96" s="319"/>
-      <c r="I96" s="319"/>
-      <c r="J96" s="319"/>
-      <c r="K96" s="319"/>
-      <c r="L96" s="320"/>
+      <c r="G96" s="315"/>
+      <c r="H96" s="315"/>
+      <c r="I96" s="315"/>
+      <c r="J96" s="315"/>
+      <c r="K96" s="315"/>
+      <c r="L96" s="316"/>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
       <c r="O96" s="10"/>
@@ -6297,7 +6297,7 @@
         <v>1</v>
       </c>
       <c r="R99" s="97"/>
-      <c r="S99" s="315"/>
+      <c r="S99" s="325"/>
     </row>
     <row r="100" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C100" s="76">
@@ -6334,7 +6334,7 @@
         <v>1</v>
       </c>
       <c r="R100" s="97"/>
-      <c r="S100" s="315"/>
+      <c r="S100" s="325"/>
     </row>
     <row r="101" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C101" s="76">
@@ -6371,7 +6371,7 @@
       <c r="P101" s="76"/>
       <c r="Q101" s="76"/>
       <c r="R101" s="97"/>
-      <c r="S101" s="315"/>
+      <c r="S101" s="325"/>
     </row>
     <row r="102" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C102" s="76">
@@ -6408,7 +6408,7 @@
         <v>1</v>
       </c>
       <c r="R102" s="97"/>
-      <c r="S102" s="315"/>
+      <c r="S102" s="325"/>
     </row>
     <row r="103" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C103" s="76">
@@ -6443,7 +6443,7 @@
         <v>1</v>
       </c>
       <c r="R103" s="97"/>
-      <c r="S103" s="315"/>
+      <c r="S103" s="325"/>
     </row>
     <row r="104" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C104" s="76">
@@ -6480,7 +6480,7 @@
       <c r="P104" s="76"/>
       <c r="Q104" s="76"/>
       <c r="R104" s="97"/>
-      <c r="S104" s="315"/>
+      <c r="S104" s="325"/>
     </row>
     <row r="105" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C105" s="95">
@@ -6517,7 +6517,7 @@
         <v>2</v>
       </c>
       <c r="R105" s="98"/>
-      <c r="S105" s="316"/>
+      <c r="S105" s="326"/>
     </row>
     <row r="106" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C106" s="76">
@@ -6548,7 +6548,7 @@
       <c r="P106" s="76"/>
       <c r="Q106" s="76"/>
       <c r="R106" s="97"/>
-      <c r="S106" s="317"/>
+      <c r="S106" s="327"/>
     </row>
     <row r="107" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C107" s="76">
@@ -6587,7 +6587,7 @@
       </c>
       <c r="Q107" s="76"/>
       <c r="R107" s="97"/>
-      <c r="S107" s="315"/>
+      <c r="S107" s="325"/>
     </row>
     <row r="108" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C108" s="76">
@@ -6624,7 +6624,7 @@
         <v>1</v>
       </c>
       <c r="R108" s="97"/>
-      <c r="S108" s="315"/>
+      <c r="S108" s="325"/>
     </row>
     <row r="109" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C109" s="76">
@@ -6659,7 +6659,7 @@
       <c r="P109" s="76"/>
       <c r="Q109" s="76"/>
       <c r="R109" s="97"/>
-      <c r="S109" s="315"/>
+      <c r="S109" s="325"/>
     </row>
     <row r="110" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C110" s="76">
@@ -6696,7 +6696,7 @@
         <v>1</v>
       </c>
       <c r="R110" s="97"/>
-      <c r="S110" s="315"/>
+      <c r="S110" s="325"/>
     </row>
     <row r="111" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C111" s="76">
@@ -6733,7 +6733,7 @@
       </c>
       <c r="Q111" s="76"/>
       <c r="R111" s="97"/>
-      <c r="S111" s="315"/>
+      <c r="S111" s="325"/>
     </row>
     <row r="112" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C112" s="95">
@@ -6768,7 +6768,7 @@
       <c r="P112" s="95"/>
       <c r="Q112" s="95"/>
       <c r="R112" s="98"/>
-      <c r="S112" s="316"/>
+      <c r="S112" s="326"/>
     </row>
     <row r="113" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C113" s="76">
@@ -6809,7 +6809,7 @@
         <v>1</v>
       </c>
       <c r="R113" s="97"/>
-      <c r="S113" s="317"/>
+      <c r="S113" s="327"/>
     </row>
     <row r="114" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C114" s="76">
@@ -6844,7 +6844,7 @@
       </c>
       <c r="Q114" s="76"/>
       <c r="R114" s="97"/>
-      <c r="S114" s="315"/>
+      <c r="S114" s="325"/>
     </row>
     <row r="115" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C115" s="76">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="Q115" s="76"/>
       <c r="R115" s="97"/>
-      <c r="S115" s="315"/>
+      <c r="S115" s="325"/>
     </row>
     <row r="116" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C116" s="76">
@@ -6914,7 +6914,7 @@
       <c r="P116" s="76"/>
       <c r="Q116" s="76"/>
       <c r="R116" s="97"/>
-      <c r="S116" s="315"/>
+      <c r="S116" s="325"/>
     </row>
     <row r="117" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C117" s="76">
@@ -6951,7 +6951,7 @@
         <v>1</v>
       </c>
       <c r="R117" s="97"/>
-      <c r="S117" s="315"/>
+      <c r="S117" s="325"/>
     </row>
     <row r="118" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C118" s="76">
@@ -6982,7 +6982,7 @@
       <c r="P118" s="76"/>
       <c r="Q118" s="76"/>
       <c r="R118" s="97"/>
-      <c r="S118" s="315"/>
+      <c r="S118" s="325"/>
     </row>
     <row r="119" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C119" s="95">
@@ -7013,7 +7013,7 @@
       <c r="P119" s="95"/>
       <c r="Q119" s="95"/>
       <c r="R119" s="98"/>
-      <c r="S119" s="316"/>
+      <c r="S119" s="326"/>
     </row>
     <row r="120" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C120" s="76">
@@ -7422,15 +7422,15 @@
       <c r="R130" s="143"/>
     </row>
     <row r="131" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="F131" s="321">
+      <c r="F131" s="320">
         <f>SUM(F130:K130)</f>
         <v>5.9270833333333321</v>
       </c>
-      <c r="G131" s="322"/>
-      <c r="H131" s="322"/>
-      <c r="I131" s="322"/>
-      <c r="J131" s="322"/>
-      <c r="K131" s="322"/>
+      <c r="G131" s="328"/>
+      <c r="H131" s="328"/>
+      <c r="I131" s="328"/>
+      <c r="J131" s="328"/>
+      <c r="K131" s="328"/>
     </row>
     <row r="133" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D133" s="5" t="s">
@@ -8677,15 +8677,15 @@
       <c r="R166" s="143"/>
     </row>
     <row r="167" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="F167" s="321">
+      <c r="F167" s="320">
         <f>SUM(F166:K166)</f>
         <v>5.0687500000000005</v>
       </c>
-      <c r="G167" s="321"/>
-      <c r="H167" s="321"/>
-      <c r="I167" s="321"/>
-      <c r="J167" s="321"/>
-      <c r="K167" s="321"/>
+      <c r="G167" s="320"/>
+      <c r="H167" s="320"/>
+      <c r="I167" s="320"/>
+      <c r="J167" s="320"/>
+      <c r="K167" s="320"/>
     </row>
     <row r="170" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="171" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9895,15 +9895,15 @@
       <c r="R202" s="101"/>
     </row>
     <row r="203" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F203" s="318">
+      <c r="F203" s="314">
         <f>SUM(F202:K202)</f>
         <v>5.4180555555555543</v>
       </c>
-      <c r="G203" s="319"/>
-      <c r="H203" s="319"/>
-      <c r="I203" s="319"/>
-      <c r="J203" s="319"/>
-      <c r="K203" s="320"/>
+      <c r="G203" s="315"/>
+      <c r="H203" s="315"/>
+      <c r="I203" s="315"/>
+      <c r="J203" s="315"/>
+      <c r="K203" s="316"/>
     </row>
     <row r="204" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C204" s="5" t="s">
@@ -10024,7 +10024,7 @@
       <c r="P207" s="61"/>
       <c r="Q207" s="61"/>
       <c r="R207" s="252"/>
-      <c r="S207" s="312">
+      <c r="S207" s="322">
         <f>SUM(O207:O213)</f>
         <v>1.3187500000000001</v>
       </c>
@@ -10068,7 +10068,7 @@
       <c r="P208" s="14"/>
       <c r="Q208" s="14"/>
       <c r="R208" s="253"/>
-      <c r="S208" s="313"/>
+      <c r="S208" s="323"/>
     </row>
     <row r="209" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C209" s="4">
@@ -10108,7 +10108,7 @@
       <c r="R209" s="253">
         <v>1</v>
       </c>
-      <c r="S209" s="313"/>
+      <c r="S209" s="323"/>
     </row>
     <row r="210" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C210" s="4">
@@ -10146,7 +10146,7 @@
       <c r="R210" s="253">
         <v>1</v>
       </c>
-      <c r="S210" s="313"/>
+      <c r="S210" s="323"/>
     </row>
     <row r="211" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C211" s="4">
@@ -10185,7 +10185,7 @@
       <c r="P211" s="14"/>
       <c r="Q211" s="14"/>
       <c r="R211" s="253"/>
-      <c r="S211" s="313"/>
+      <c r="S211" s="323"/>
     </row>
     <row r="212" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C212" s="4">
@@ -10226,7 +10226,7 @@
       </c>
       <c r="Q212" s="14"/>
       <c r="R212" s="253"/>
-      <c r="S212" s="313"/>
+      <c r="S212" s="323"/>
     </row>
     <row r="213" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C213" s="4">
@@ -10269,7 +10269,7 @@
       <c r="R213" s="253">
         <v>1</v>
       </c>
-      <c r="S213" s="314"/>
+      <c r="S213" s="324"/>
     </row>
     <row r="214" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C214" s="4">
@@ -10310,7 +10310,7 @@
       <c r="P214" s="14"/>
       <c r="Q214" s="14"/>
       <c r="R214" s="253"/>
-      <c r="S214" s="312">
+      <c r="S214" s="322">
         <f>SUM(O214:O220)</f>
         <v>1.2152777777777777</v>
       </c>
@@ -10356,7 +10356,7 @@
       </c>
       <c r="Q215" s="14"/>
       <c r="R215" s="253"/>
-      <c r="S215" s="313"/>
+      <c r="S215" s="323"/>
     </row>
     <row r="216" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C216" s="4">
@@ -10397,7 +10397,7 @@
       <c r="R216" s="253">
         <v>1</v>
       </c>
-      <c r="S216" s="313"/>
+      <c r="S216" s="323"/>
     </row>
     <row r="217" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C217" s="4">
@@ -10438,7 +10438,7 @@
       </c>
       <c r="Q217" s="14"/>
       <c r="R217" s="253"/>
-      <c r="S217" s="313"/>
+      <c r="S217" s="323"/>
     </row>
     <row r="218" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C218" s="4">
@@ -10481,7 +10481,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="R218" s="253"/>
-      <c r="S218" s="313"/>
+      <c r="S218" s="323"/>
     </row>
     <row r="219" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C219" s="4">
@@ -10518,15 +10518,13 @@
       <c r="P219" s="14"/>
       <c r="Q219" s="14"/>
       <c r="R219" s="253"/>
-      <c r="S219" s="313"/>
+      <c r="S219" s="323"/>
     </row>
     <row r="220" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C220" s="4">
         <v>14</v>
       </c>
-      <c r="D220" s="14">
-        <v>0.1673611111111111</v>
-      </c>
+      <c r="D220" s="14"/>
       <c r="E220" s="14"/>
       <c r="F220" s="14">
         <v>5.5555555555555552E-2</v>
@@ -10559,7 +10557,7 @@
         <v>0.11388888888888889</v>
       </c>
       <c r="R220" s="253"/>
-      <c r="S220" s="314"/>
+      <c r="S220" s="324"/>
     </row>
     <row r="221" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C221" s="4">
@@ -10598,7 +10596,7 @@
       </c>
       <c r="Q221" s="14"/>
       <c r="R221" s="253"/>
-      <c r="S221" s="312">
+      <c r="S221" s="322">
         <f>SUM(O221:O227)</f>
         <v>0.35416666666666669</v>
       </c>
@@ -10640,7 +10638,7 @@
       </c>
       <c r="Q222" s="14"/>
       <c r="R222" s="253"/>
-      <c r="S222" s="313"/>
+      <c r="S222" s="323"/>
     </row>
     <row r="223" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C223" s="4">
@@ -10681,7 +10679,7 @@
       <c r="R223" s="253">
         <v>1</v>
       </c>
-      <c r="S223" s="313"/>
+      <c r="S223" s="323"/>
     </row>
     <row r="224" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C224" s="4">
@@ -10714,7 +10712,7 @@
         <v>0.31597222222222221</v>
       </c>
       <c r="R224" s="253"/>
-      <c r="S224" s="313"/>
+      <c r="S224" s="323"/>
     </row>
     <row r="225" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C225" s="4">
@@ -10751,7 +10749,7 @@
       <c r="R225" s="253">
         <v>1</v>
       </c>
-      <c r="S225" s="313"/>
+      <c r="S225" s="323"/>
     </row>
     <row r="226" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C226" s="4">
@@ -10780,7 +10778,7 @@
       </c>
       <c r="Q226" s="14"/>
       <c r="R226" s="253"/>
-      <c r="S226" s="313"/>
+      <c r="S226" s="323"/>
     </row>
     <row r="227" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C227" s="4">
@@ -10807,7 +10805,7 @@
       </c>
       <c r="Q227" s="14"/>
       <c r="R227" s="253"/>
-      <c r="S227" s="314"/>
+      <c r="S227" s="324"/>
     </row>
     <row r="228" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C228" s="4">
@@ -11037,7 +11035,7 @@
       <c r="C238" s="99"/>
       <c r="D238" s="142">
         <f t="shared" ref="D238:J238" si="7">SUM(D207:D236)</f>
-        <v>6.3465277777777782</v>
+        <v>6.1791666666666671</v>
       </c>
       <c r="E238" s="142">
         <f t="shared" si="7"/>
@@ -11092,23 +11090,17 @@
       <c r="C239" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F239" s="311">
+      <c r="F239" s="321">
         <v>10.833333333333334</v>
       </c>
-      <c r="G239" s="311"/>
-      <c r="H239" s="311"/>
-      <c r="I239" s="311"/>
-      <c r="J239" s="311"/>
-      <c r="K239" s="311"/>
+      <c r="G239" s="321"/>
+      <c r="H239" s="321"/>
+      <c r="I239" s="321"/>
+      <c r="J239" s="321"/>
+      <c r="K239" s="321"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F96:L96"/>
-    <mergeCell ref="R65:R71"/>
-    <mergeCell ref="R72:R78"/>
-    <mergeCell ref="R79:R85"/>
-    <mergeCell ref="F61:L61"/>
     <mergeCell ref="F239:K239"/>
     <mergeCell ref="S207:S213"/>
     <mergeCell ref="S99:S105"/>
@@ -11119,6 +11111,12 @@
     <mergeCell ref="F131:K131"/>
     <mergeCell ref="S214:S220"/>
     <mergeCell ref="S221:S227"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F96:L96"/>
+    <mergeCell ref="R65:R71"/>
+    <mergeCell ref="R72:R78"/>
+    <mergeCell ref="R79:R85"/>
+    <mergeCell ref="F61:L61"/>
   </mergeCells>
   <conditionalFormatting sqref="G7">
     <cfRule type="iconSet" priority="2">
@@ -11571,15 +11569,15 @@
       <c r="C21" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="329">
+      <c r="D21" s="338">
         <f>SUM(D20:I20)</f>
         <v>7.9861111111111105E-2</v>
       </c>
-      <c r="E21" s="329"/>
-      <c r="F21" s="329"/>
-      <c r="G21" s="329"/>
-      <c r="H21" s="329"/>
-      <c r="I21" s="329"/>
+      <c r="E21" s="338"/>
+      <c r="F21" s="338"/>
+      <c r="G21" s="338"/>
+      <c r="H21" s="338"/>
+      <c r="I21" s="338"/>
       <c r="J21" s="113">
         <f>SUM(J20)</f>
         <v>4.7222222222222221E-2</v>
@@ -11587,16 +11585,16 @@
       <c r="K21" s="250"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="D22" s="330">
+      <c r="D22" s="339">
         <f>SUM(D21:J21)</f>
         <v>0.12708333333333333</v>
       </c>
-      <c r="E22" s="331"/>
-      <c r="F22" s="331"/>
-      <c r="G22" s="331"/>
-      <c r="H22" s="331"/>
-      <c r="I22" s="331"/>
-      <c r="J22" s="331"/>
+      <c r="E22" s="340"/>
+      <c r="F22" s="340"/>
+      <c r="G22" s="340"/>
+      <c r="H22" s="340"/>
+      <c r="I22" s="340"/>
+      <c r="J22" s="340"/>
       <c r="K22" s="251"/>
       <c r="L22" s="22"/>
     </row>
@@ -11607,96 +11605,96 @@
     </row>
     <row r="24" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="332" t="s">
+      <c r="C25" s="341" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="333"/>
-      <c r="E25" s="333"/>
-      <c r="F25" s="333"/>
-      <c r="G25" s="333"/>
-      <c r="H25" s="333"/>
-      <c r="I25" s="334"/>
+      <c r="D25" s="342"/>
+      <c r="E25" s="342"/>
+      <c r="F25" s="342"/>
+      <c r="G25" s="342"/>
+      <c r="H25" s="342"/>
+      <c r="I25" s="343"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C26" s="335"/>
-      <c r="D26" s="336"/>
-      <c r="E26" s="336"/>
-      <c r="F26" s="336"/>
-      <c r="G26" s="336"/>
-      <c r="H26" s="336"/>
-      <c r="I26" s="337"/>
+      <c r="C26" s="344"/>
+      <c r="D26" s="345"/>
+      <c r="E26" s="345"/>
+      <c r="F26" s="345"/>
+      <c r="G26" s="345"/>
+      <c r="H26" s="345"/>
+      <c r="I26" s="346"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C27" s="338"/>
-      <c r="D27" s="339"/>
-      <c r="E27" s="339"/>
-      <c r="F27" s="339"/>
-      <c r="G27" s="339"/>
-      <c r="H27" s="339"/>
-      <c r="I27" s="340"/>
+      <c r="C27" s="335"/>
+      <c r="D27" s="336"/>
+      <c r="E27" s="336"/>
+      <c r="F27" s="336"/>
+      <c r="G27" s="336"/>
+      <c r="H27" s="336"/>
+      <c r="I27" s="337"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C28" s="338"/>
-      <c r="D28" s="339"/>
-      <c r="E28" s="339"/>
-      <c r="F28" s="339"/>
-      <c r="G28" s="339"/>
-      <c r="H28" s="339"/>
-      <c r="I28" s="340"/>
+      <c r="C28" s="335"/>
+      <c r="D28" s="336"/>
+      <c r="E28" s="336"/>
+      <c r="F28" s="336"/>
+      <c r="G28" s="336"/>
+      <c r="H28" s="336"/>
+      <c r="I28" s="337"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C29" s="341"/>
-      <c r="D29" s="342"/>
-      <c r="E29" s="342"/>
-      <c r="F29" s="342"/>
-      <c r="G29" s="342"/>
-      <c r="H29" s="342"/>
-      <c r="I29" s="343"/>
+      <c r="C29" s="329"/>
+      <c r="D29" s="330"/>
+      <c r="E29" s="330"/>
+      <c r="F29" s="330"/>
+      <c r="G29" s="330"/>
+      <c r="H29" s="330"/>
+      <c r="I29" s="331"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C30" s="341"/>
-      <c r="D30" s="342"/>
-      <c r="E30" s="342"/>
-      <c r="F30" s="342"/>
-      <c r="G30" s="342"/>
-      <c r="H30" s="342"/>
-      <c r="I30" s="343"/>
+      <c r="C30" s="329"/>
+      <c r="D30" s="330"/>
+      <c r="E30" s="330"/>
+      <c r="F30" s="330"/>
+      <c r="G30" s="330"/>
+      <c r="H30" s="330"/>
+      <c r="I30" s="331"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C31" s="341"/>
-      <c r="D31" s="342"/>
-      <c r="E31" s="342"/>
-      <c r="F31" s="342"/>
-      <c r="G31" s="342"/>
-      <c r="H31" s="342"/>
-      <c r="I31" s="343"/>
+      <c r="C31" s="329"/>
+      <c r="D31" s="330"/>
+      <c r="E31" s="330"/>
+      <c r="F31" s="330"/>
+      <c r="G31" s="330"/>
+      <c r="H31" s="330"/>
+      <c r="I31" s="331"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C32" s="341"/>
-      <c r="D32" s="342"/>
-      <c r="E32" s="342"/>
-      <c r="F32" s="342"/>
-      <c r="G32" s="342"/>
-      <c r="H32" s="342"/>
-      <c r="I32" s="343"/>
+      <c r="C32" s="329"/>
+      <c r="D32" s="330"/>
+      <c r="E32" s="330"/>
+      <c r="F32" s="330"/>
+      <c r="G32" s="330"/>
+      <c r="H32" s="330"/>
+      <c r="I32" s="331"/>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="C33" s="341"/>
-      <c r="D33" s="342"/>
-      <c r="E33" s="342"/>
-      <c r="F33" s="342"/>
-      <c r="G33" s="342"/>
-      <c r="H33" s="342"/>
-      <c r="I33" s="343"/>
+      <c r="C33" s="329"/>
+      <c r="D33" s="330"/>
+      <c r="E33" s="330"/>
+      <c r="F33" s="330"/>
+      <c r="G33" s="330"/>
+      <c r="H33" s="330"/>
+      <c r="I33" s="331"/>
     </row>
     <row r="34" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="344"/>
-      <c r="D34" s="345"/>
-      <c r="E34" s="345"/>
-      <c r="F34" s="345"/>
-      <c r="G34" s="345"/>
-      <c r="H34" s="345"/>
-      <c r="I34" s="346"/>
+      <c r="C34" s="332"/>
+      <c r="D34" s="333"/>
+      <c r="E34" s="333"/>
+      <c r="F34" s="333"/>
+      <c r="G34" s="333"/>
+      <c r="H34" s="333"/>
+      <c r="I34" s="334"/>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C35" s="151"/>
@@ -11827,6 +11825,11 @@
     <sortCondition descending="1" ref="H12"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
     <mergeCell ref="C33:I33"/>
     <mergeCell ref="C34:I34"/>
     <mergeCell ref="C28:I28"/>
@@ -11834,11 +11837,6 @@
     <mergeCell ref="C30:I30"/>
     <mergeCell ref="C31:I31"/>
     <mergeCell ref="C32:I32"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D22:J22"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -14519,7 +14517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54DCEE8-36D1-4DB4-AB83-DE623461528D}">
   <dimension ref="A1:K285"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -14544,15 +14542,15 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="352" t="s">
+      <c r="B3" s="413" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="352"/>
+      <c r="C3" s="413"/>
       <c r="D3" s="16"/>
-      <c r="F3" s="405" t="s">
+      <c r="F3" s="377" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="405"/>
+      <c r="G3" s="377"/>
       <c r="H3" s="274"/>
       <c r="I3" s="274"/>
       <c r="J3" s="149"/>
@@ -14561,10 +14559,10 @@
       <c r="B4" s="238" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="381" t="s">
+      <c r="C4" s="404" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="382"/>
+      <c r="D4" s="405"/>
       <c r="F4" s="273" t="s">
         <v>204</v>
       </c>
@@ -14582,17 +14580,17 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="359" t="s">
+      <c r="B5" s="382" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="388">
+      <c r="C5" s="411">
         <v>1</v>
       </c>
-      <c r="D5" s="390"/>
-      <c r="F5" s="411" t="s">
+      <c r="D5" s="412"/>
+      <c r="F5" s="358" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="410">
+      <c r="G5" s="364">
         <v>22</v>
       </c>
       <c r="H5" s="295" t="s">
@@ -14603,13 +14601,13 @@
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="360"/>
-      <c r="C6" s="383" t="s">
+      <c r="B6" s="383"/>
+      <c r="C6" s="406" t="s">
         <v>212</v>
       </c>
-      <c r="D6" s="384"/>
-      <c r="F6" s="412"/>
-      <c r="G6" s="401"/>
+      <c r="D6" s="407"/>
+      <c r="F6" s="359"/>
+      <c r="G6" s="365"/>
       <c r="H6" s="296" t="s">
         <v>60</v>
       </c>
@@ -14619,13 +14617,13 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="360"/>
-      <c r="C7" s="385">
+      <c r="B7" s="383"/>
+      <c r="C7" s="408">
         <v>2</v>
       </c>
-      <c r="D7" s="370"/>
-      <c r="F7" s="412"/>
-      <c r="G7" s="401"/>
+      <c r="D7" s="393"/>
+      <c r="F7" s="359"/>
+      <c r="G7" s="365"/>
       <c r="H7" s="296" t="s">
         <v>16</v>
       </c>
@@ -14635,13 +14633,13 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="360"/>
-      <c r="C8" s="383" t="s">
+      <c r="B8" s="383"/>
+      <c r="C8" s="406" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="384"/>
-      <c r="F8" s="412"/>
-      <c r="G8" s="401"/>
+      <c r="D8" s="407"/>
+      <c r="F8" s="359"/>
+      <c r="G8" s="365"/>
       <c r="H8" s="296" t="s">
         <v>8</v>
       </c>
@@ -14649,13 +14647,13 @@
       <c r="J8" s="190"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="360"/>
-      <c r="C9" s="386">
+      <c r="B9" s="383"/>
+      <c r="C9" s="409">
         <v>3</v>
       </c>
-      <c r="D9" s="387"/>
-      <c r="F9" s="412"/>
-      <c r="G9" s="401"/>
+      <c r="D9" s="410"/>
+      <c r="F9" s="359"/>
+      <c r="G9" s="365"/>
       <c r="H9" s="296" t="s">
         <v>162</v>
       </c>
@@ -14665,16 +14663,16 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="361"/>
-      <c r="C10" s="383" t="s">
+      <c r="B10" s="384"/>
+      <c r="C10" s="406" t="s">
         <v>217</v>
       </c>
-      <c r="D10" s="384"/>
+      <c r="D10" s="407"/>
       <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="412"/>
-      <c r="G10" s="401"/>
+      <c r="F10" s="359"/>
+      <c r="G10" s="365"/>
       <c r="H10" s="296" t="s">
         <v>6</v>
       </c>
@@ -14684,25 +14682,25 @@
       </c>
     </row>
     <row r="11" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="359" t="s">
+      <c r="B11" s="382" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="388"/>
-      <c r="D11" s="389"/>
-      <c r="F11" s="412"/>
-      <c r="G11" s="402"/>
+      <c r="C11" s="411"/>
+      <c r="D11" s="390"/>
+      <c r="F11" s="359"/>
+      <c r="G11" s="366"/>
       <c r="H11" s="297"/>
       <c r="I11" s="300"/>
       <c r="J11" s="190"/>
     </row>
     <row r="12" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="360"/>
-      <c r="C12" s="368" t="s">
+      <c r="B12" s="383"/>
+      <c r="C12" s="375" t="s">
         <v>169</v>
       </c>
-      <c r="D12" s="340"/>
-      <c r="F12" s="412"/>
-      <c r="G12" s="414">
+      <c r="D12" s="337"/>
+      <c r="F12" s="359"/>
+      <c r="G12" s="361">
         <v>23</v>
       </c>
       <c r="H12" s="304" t="s">
@@ -14716,11 +14714,11 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="360"/>
-      <c r="C13" s="368"/>
-      <c r="D13" s="340"/>
-      <c r="F13" s="412"/>
-      <c r="G13" s="393"/>
+      <c r="B13" s="383"/>
+      <c r="C13" s="375"/>
+      <c r="D13" s="337"/>
+      <c r="F13" s="359"/>
+      <c r="G13" s="362"/>
       <c r="H13" s="306" t="s">
         <v>60</v>
       </c>
@@ -14730,11 +14728,11 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="360"/>
-      <c r="C14" s="368"/>
-      <c r="D14" s="340"/>
-      <c r="F14" s="412"/>
-      <c r="G14" s="393"/>
+      <c r="B14" s="383"/>
+      <c r="C14" s="375"/>
+      <c r="D14" s="337"/>
+      <c r="F14" s="359"/>
+      <c r="G14" s="362"/>
       <c r="H14" s="306" t="s">
         <v>16</v>
       </c>
@@ -14742,11 +14740,11 @@
       <c r="J14" s="188"/>
     </row>
     <row r="15" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="360"/>
-      <c r="C15" s="368"/>
-      <c r="D15" s="340"/>
-      <c r="F15" s="412"/>
-      <c r="G15" s="393"/>
+      <c r="B15" s="383"/>
+      <c r="C15" s="375"/>
+      <c r="D15" s="337"/>
+      <c r="F15" s="359"/>
+      <c r="G15" s="362"/>
       <c r="H15" s="306" t="s">
         <v>8</v>
       </c>
@@ -14754,11 +14752,11 @@
       <c r="J15" s="190"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="360"/>
-      <c r="C16" s="368"/>
-      <c r="D16" s="340"/>
-      <c r="F16" s="412"/>
-      <c r="G16" s="393"/>
+      <c r="B16" s="383"/>
+      <c r="C16" s="375"/>
+      <c r="D16" s="337"/>
+      <c r="F16" s="359"/>
+      <c r="G16" s="362"/>
       <c r="H16" s="306" t="s">
         <v>162</v>
       </c>
@@ -14770,11 +14768,11 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="361"/>
-      <c r="C17" s="374"/>
-      <c r="D17" s="375"/>
-      <c r="F17" s="412"/>
-      <c r="G17" s="393"/>
+      <c r="B17" s="384"/>
+      <c r="C17" s="418"/>
+      <c r="D17" s="419"/>
+      <c r="F17" s="359"/>
+      <c r="G17" s="362"/>
       <c r="H17" s="306" t="s">
         <v>6</v>
       </c>
@@ -14784,27 +14782,27 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="359" t="s">
+      <c r="B18" s="382" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="409" t="s">
+      <c r="C18" s="389" t="s">
         <v>197</v>
       </c>
-      <c r="D18" s="389"/>
-      <c r="F18" s="412"/>
-      <c r="G18" s="404"/>
+      <c r="D18" s="390"/>
+      <c r="F18" s="359"/>
+      <c r="G18" s="363"/>
       <c r="H18" s="309"/>
       <c r="I18" s="310"/>
       <c r="J18" s="190"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="360"/>
-      <c r="C19" s="373" t="s">
+      <c r="B19" s="383"/>
+      <c r="C19" s="372" t="s">
         <v>199</v>
       </c>
-      <c r="D19" s="363"/>
-      <c r="F19" s="412"/>
-      <c r="G19" s="410">
+      <c r="D19" s="373"/>
+      <c r="F19" s="359"/>
+      <c r="G19" s="364">
         <v>24</v>
       </c>
       <c r="H19" s="295" t="s">
@@ -14818,11 +14816,11 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="360"/>
-      <c r="C20" s="368"/>
-      <c r="D20" s="340"/>
-      <c r="F20" s="412"/>
-      <c r="G20" s="401"/>
+      <c r="B20" s="383"/>
+      <c r="C20" s="375"/>
+      <c r="D20" s="337"/>
+      <c r="F20" s="359"/>
+      <c r="G20" s="365"/>
       <c r="H20" s="296" t="s">
         <v>60</v>
       </c>
@@ -14832,11 +14830,11 @@
       </c>
     </row>
     <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="361"/>
-      <c r="C21" s="416"/>
-      <c r="D21" s="365"/>
-      <c r="F21" s="412"/>
-      <c r="G21" s="401"/>
+      <c r="B21" s="384"/>
+      <c r="C21" s="374"/>
+      <c r="D21" s="371"/>
+      <c r="F21" s="359"/>
+      <c r="G21" s="365"/>
       <c r="H21" s="296" t="s">
         <v>16</v>
       </c>
@@ -14846,13 +14844,13 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="359" t="s">
+      <c r="B22" s="382" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="371"/>
-      <c r="D22" s="372"/>
-      <c r="F22" s="412"/>
-      <c r="G22" s="401"/>
+      <c r="C22" s="368"/>
+      <c r="D22" s="369"/>
+      <c r="F22" s="359"/>
+      <c r="G22" s="365"/>
       <c r="H22" s="296" t="s">
         <v>8</v>
       </c>
@@ -14860,11 +14858,11 @@
       <c r="J22" s="188"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="360"/>
-      <c r="C23" s="362"/>
-      <c r="D23" s="363"/>
-      <c r="F23" s="412"/>
-      <c r="G23" s="401"/>
+      <c r="B23" s="383"/>
+      <c r="C23" s="376"/>
+      <c r="D23" s="373"/>
+      <c r="F23" s="359"/>
+      <c r="G23" s="365"/>
       <c r="H23" s="296" t="s">
         <v>162</v>
       </c>
@@ -14872,11 +14870,11 @@
       <c r="J23" s="188"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="360"/>
-      <c r="C24" s="362"/>
-      <c r="D24" s="363"/>
-      <c r="F24" s="412"/>
-      <c r="G24" s="401"/>
+      <c r="B24" s="383"/>
+      <c r="C24" s="376"/>
+      <c r="D24" s="373"/>
+      <c r="F24" s="359"/>
+      <c r="G24" s="365"/>
       <c r="H24" s="296" t="s">
         <v>6</v>
       </c>
@@ -14884,21 +14882,21 @@
       <c r="J24" s="188"/>
     </row>
     <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="360"/>
-      <c r="C25" s="362"/>
-      <c r="D25" s="363"/>
-      <c r="F25" s="412"/>
-      <c r="G25" s="402"/>
+      <c r="B25" s="383"/>
+      <c r="C25" s="376"/>
+      <c r="D25" s="373"/>
+      <c r="F25" s="359"/>
+      <c r="G25" s="366"/>
       <c r="H25" s="297"/>
       <c r="I25" s="302"/>
       <c r="J25" s="188"/>
     </row>
     <row r="26" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="361"/>
-      <c r="C26" s="364"/>
-      <c r="D26" s="365"/>
-      <c r="F26" s="412"/>
-      <c r="G26" s="410">
+      <c r="B26" s="384"/>
+      <c r="C26" s="370"/>
+      <c r="D26" s="371"/>
+      <c r="F26" s="359"/>
+      <c r="G26" s="364">
         <v>25</v>
       </c>
       <c r="H26" s="295" t="s">
@@ -14910,13 +14908,13 @@
       <c r="J26" s="188"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="359" t="s">
+      <c r="B27" s="382" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="371"/>
-      <c r="D27" s="372"/>
-      <c r="F27" s="412"/>
-      <c r="G27" s="401"/>
+      <c r="C27" s="368"/>
+      <c r="D27" s="369"/>
+      <c r="F27" s="359"/>
+      <c r="G27" s="365"/>
       <c r="H27" s="296" t="s">
         <v>60</v>
       </c>
@@ -14924,13 +14922,13 @@
       <c r="J27" s="188"/>
     </row>
     <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="361"/>
-      <c r="C28" s="364" t="s">
+      <c r="B28" s="384"/>
+      <c r="C28" s="370" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="365"/>
-      <c r="F28" s="412"/>
-      <c r="G28" s="401"/>
+      <c r="D28" s="371"/>
+      <c r="F28" s="359"/>
+      <c r="G28" s="365"/>
       <c r="H28" s="296" t="s">
         <v>16</v>
       </c>
@@ -14938,15 +14936,15 @@
       <c r="J28" s="188"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="359" t="s">
+      <c r="B29" s="382" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="366" t="s">
+      <c r="C29" s="416" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="367"/>
-      <c r="F29" s="412"/>
-      <c r="G29" s="401"/>
+      <c r="D29" s="417"/>
+      <c r="F29" s="359"/>
+      <c r="G29" s="365"/>
       <c r="H29" s="296" t="s">
         <v>8</v>
       </c>
@@ -14954,11 +14952,11 @@
       <c r="J29" s="188"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="360"/>
-      <c r="C30" s="373"/>
-      <c r="D30" s="363"/>
-      <c r="F30" s="412"/>
-      <c r="G30" s="401"/>
+      <c r="B30" s="383"/>
+      <c r="C30" s="372"/>
+      <c r="D30" s="373"/>
+      <c r="F30" s="359"/>
+      <c r="G30" s="365"/>
       <c r="H30" s="296" t="s">
         <v>162</v>
       </c>
@@ -14966,11 +14964,11 @@
       <c r="J30" s="188"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="360"/>
-      <c r="C31" s="373"/>
-      <c r="D31" s="363"/>
-      <c r="F31" s="412"/>
-      <c r="G31" s="401"/>
+      <c r="B31" s="383"/>
+      <c r="C31" s="372"/>
+      <c r="D31" s="373"/>
+      <c r="F31" s="359"/>
+      <c r="G31" s="365"/>
       <c r="H31" s="296" t="s">
         <v>6</v>
       </c>
@@ -14978,23 +14976,23 @@
       <c r="J31" s="188"/>
     </row>
     <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="360"/>
-      <c r="C32" s="369" t="s">
+      <c r="B32" s="383"/>
+      <c r="C32" s="392" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="370"/>
-      <c r="F32" s="412"/>
-      <c r="G32" s="402"/>
+      <c r="D32" s="393"/>
+      <c r="F32" s="359"/>
+      <c r="G32" s="366"/>
       <c r="H32" s="297"/>
       <c r="I32" s="302"/>
       <c r="J32" s="188"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="360"/>
-      <c r="C33" s="373"/>
-      <c r="D33" s="363"/>
-      <c r="F33" s="412"/>
-      <c r="G33" s="410">
+      <c r="B33" s="383"/>
+      <c r="C33" s="372"/>
+      <c r="D33" s="373"/>
+      <c r="F33" s="359"/>
+      <c r="G33" s="364">
         <v>26</v>
       </c>
       <c r="H33" s="295" t="s">
@@ -15006,11 +15004,11 @@
       <c r="J33" s="188"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="360"/>
-      <c r="C34" s="373"/>
-      <c r="D34" s="363"/>
-      <c r="F34" s="412"/>
-      <c r="G34" s="401"/>
+      <c r="B34" s="383"/>
+      <c r="C34" s="372"/>
+      <c r="D34" s="373"/>
+      <c r="F34" s="359"/>
+      <c r="G34" s="365"/>
       <c r="H34" s="296" t="s">
         <v>60</v>
       </c>
@@ -15018,11 +15016,11 @@
       <c r="J34" s="188"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="360"/>
-      <c r="C35" s="369"/>
-      <c r="D35" s="370"/>
-      <c r="F35" s="412"/>
-      <c r="G35" s="401"/>
+      <c r="B35" s="383"/>
+      <c r="C35" s="392"/>
+      <c r="D35" s="393"/>
+      <c r="F35" s="359"/>
+      <c r="G35" s="365"/>
       <c r="H35" s="296" t="s">
         <v>16</v>
       </c>
@@ -15030,11 +15028,11 @@
       <c r="J35" s="188"/>
     </row>
     <row r="36" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="361"/>
-      <c r="C36" s="364"/>
-      <c r="D36" s="365"/>
-      <c r="F36" s="412"/>
-      <c r="G36" s="401"/>
+      <c r="B36" s="384"/>
+      <c r="C36" s="370"/>
+      <c r="D36" s="371"/>
+      <c r="F36" s="359"/>
+      <c r="G36" s="365"/>
       <c r="H36" s="296" t="s">
         <v>8</v>
       </c>
@@ -15042,15 +15040,15 @@
       <c r="J36" s="188"/>
     </row>
     <row r="37" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="359" t="s">
+      <c r="B37" s="382" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="371" t="s">
+      <c r="C37" s="368" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="372"/>
-      <c r="F37" s="412"/>
-      <c r="G37" s="401"/>
+      <c r="D37" s="369"/>
+      <c r="F37" s="359"/>
+      <c r="G37" s="365"/>
       <c r="H37" s="296" t="s">
         <v>162</v>
       </c>
@@ -15058,13 +15056,13 @@
       <c r="J37" s="188"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="360"/>
-      <c r="C38" s="373" t="s">
+      <c r="B38" s="383"/>
+      <c r="C38" s="372" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="363"/>
-      <c r="F38" s="412"/>
-      <c r="G38" s="401"/>
+      <c r="D38" s="373"/>
+      <c r="F38" s="359"/>
+      <c r="G38" s="365"/>
       <c r="H38" s="296" t="s">
         <v>6</v>
       </c>
@@ -15072,18 +15070,18 @@
       <c r="J38" s="188"/>
     </row>
     <row r="39" spans="2:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="361"/>
-      <c r="C39" s="364"/>
-      <c r="D39" s="365"/>
-      <c r="F39" s="412"/>
-      <c r="G39" s="415"/>
+      <c r="B39" s="384"/>
+      <c r="C39" s="370"/>
+      <c r="D39" s="371"/>
+      <c r="F39" s="359"/>
+      <c r="G39" s="367"/>
       <c r="H39" s="297"/>
       <c r="I39" s="303"/>
       <c r="J39" s="188"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="412"/>
-      <c r="G40" s="410">
+      <c r="F40" s="359"/>
+      <c r="G40" s="364">
         <v>27</v>
       </c>
       <c r="H40" s="295" t="s">
@@ -15095,8 +15093,8 @@
       <c r="J40" s="188"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F41" s="412"/>
-      <c r="G41" s="401"/>
+      <c r="F41" s="359"/>
+      <c r="G41" s="365"/>
       <c r="H41" s="296" t="s">
         <v>60</v>
       </c>
@@ -15104,8 +15102,8 @@
       <c r="J41" s="188"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F42" s="412"/>
-      <c r="G42" s="401"/>
+      <c r="F42" s="359"/>
+      <c r="G42" s="365"/>
       <c r="H42" s="296" t="s">
         <v>16</v>
       </c>
@@ -15113,8 +15111,8 @@
       <c r="J42" s="188"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F43" s="412"/>
-      <c r="G43" s="401"/>
+      <c r="F43" s="359"/>
+      <c r="G43" s="365"/>
       <c r="H43" s="296" t="s">
         <v>8</v>
       </c>
@@ -15125,8 +15123,8 @@
       <c r="C44" s="160"/>
       <c r="D44" s="149"/>
       <c r="E44" s="149"/>
-      <c r="F44" s="412"/>
-      <c r="G44" s="401"/>
+      <c r="F44" s="359"/>
+      <c r="G44" s="365"/>
       <c r="H44" s="296" t="s">
         <v>162</v>
       </c>
@@ -15135,8 +15133,8 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E45" s="149"/>
-      <c r="F45" s="412"/>
-      <c r="G45" s="401"/>
+      <c r="F45" s="359"/>
+      <c r="G45" s="365"/>
       <c r="H45" s="296" t="s">
         <v>6</v>
       </c>
@@ -15145,16 +15143,16 @@
     </row>
     <row r="46" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E46" s="149"/>
-      <c r="F46" s="412"/>
-      <c r="G46" s="402"/>
+      <c r="F46" s="359"/>
+      <c r="G46" s="366"/>
       <c r="H46" s="297"/>
       <c r="I46" s="302"/>
       <c r="J46" s="188"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E47" s="149"/>
-      <c r="F47" s="412"/>
-      <c r="G47" s="410">
+      <c r="F47" s="359"/>
+      <c r="G47" s="364">
         <v>28</v>
       </c>
       <c r="H47" s="295" t="s">
@@ -15167,8 +15165,8 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E48" s="149"/>
-      <c r="F48" s="412"/>
-      <c r="G48" s="401"/>
+      <c r="F48" s="359"/>
+      <c r="G48" s="365"/>
       <c r="H48" s="296" t="s">
         <v>60</v>
       </c>
@@ -15177,8 +15175,8 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E49" s="149"/>
-      <c r="F49" s="412"/>
-      <c r="G49" s="401"/>
+      <c r="F49" s="359"/>
+      <c r="G49" s="365"/>
       <c r="H49" s="296" t="s">
         <v>16</v>
       </c>
@@ -15187,8 +15185,8 @@
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E50" s="149"/>
-      <c r="F50" s="412"/>
-      <c r="G50" s="401"/>
+      <c r="F50" s="359"/>
+      <c r="G50" s="365"/>
       <c r="H50" s="296" t="s">
         <v>8</v>
       </c>
@@ -15197,8 +15195,8 @@
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E51" s="149"/>
-      <c r="F51" s="412"/>
-      <c r="G51" s="401"/>
+      <c r="F51" s="359"/>
+      <c r="G51" s="365"/>
       <c r="H51" s="296" t="s">
         <v>162</v>
       </c>
@@ -15207,8 +15205,8 @@
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E52" s="149"/>
-      <c r="F52" s="412"/>
-      <c r="G52" s="401"/>
+      <c r="F52" s="359"/>
+      <c r="G52" s="365"/>
       <c r="H52" s="296" t="s">
         <v>6</v>
       </c>
@@ -15217,8 +15215,8 @@
     </row>
     <row r="53" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E53" s="149"/>
-      <c r="F53" s="413"/>
-      <c r="G53" s="402"/>
+      <c r="F53" s="360"/>
+      <c r="G53" s="366"/>
       <c r="H53" s="297"/>
       <c r="I53" s="300"/>
       <c r="J53" s="294"/>
@@ -15288,8 +15286,8 @@
       <c r="J61" s="291"/>
     </row>
     <row r="62" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="352"/>
-      <c r="C62" s="352"/>
+      <c r="B62" s="413"/>
+      <c r="C62" s="413"/>
       <c r="E62" s="149"/>
       <c r="F62" s="185"/>
       <c r="G62" s="185"/>
@@ -15301,10 +15299,10 @@
       <c r="B63" s="239" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="353" t="s">
+      <c r="C63" s="414" t="s">
         <v>70</v>
       </c>
-      <c r="D63" s="354"/>
+      <c r="D63" s="415"/>
       <c r="E63" s="149"/>
       <c r="F63" s="185"/>
       <c r="G63" s="185"/>
@@ -15313,11 +15311,11 @@
       <c r="J63" s="291"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B64" s="376" t="s">
+      <c r="B64" s="394" t="s">
         <v>38</v>
       </c>
-      <c r="C64" s="355"/>
-      <c r="D64" s="356"/>
+      <c r="C64" s="397"/>
+      <c r="D64" s="398"/>
       <c r="E64" s="149"/>
       <c r="F64" s="185"/>
       <c r="G64" s="185"/>
@@ -15326,9 +15324,9 @@
       <c r="J64" s="291"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B65" s="377"/>
-      <c r="C65" s="357"/>
-      <c r="D65" s="358"/>
+      <c r="B65" s="395"/>
+      <c r="C65" s="399"/>
+      <c r="D65" s="400"/>
       <c r="E65" s="149"/>
       <c r="F65" s="185"/>
       <c r="G65" s="185"/>
@@ -15337,9 +15335,9 @@
       <c r="J65" s="291"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B66" s="377"/>
-      <c r="C66" s="357"/>
-      <c r="D66" s="358"/>
+      <c r="B66" s="395"/>
+      <c r="C66" s="399"/>
+      <c r="D66" s="400"/>
       <c r="E66" s="149"/>
       <c r="F66" s="185"/>
       <c r="G66" s="185"/>
@@ -15348,9 +15346,9 @@
       <c r="J66" s="291"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B67" s="377"/>
-      <c r="C67" s="357"/>
-      <c r="D67" s="358"/>
+      <c r="B67" s="395"/>
+      <c r="C67" s="399"/>
+      <c r="D67" s="400"/>
       <c r="E67" s="149"/>
       <c r="F67" s="185"/>
       <c r="G67" s="185"/>
@@ -15359,9 +15357,9 @@
       <c r="J67" s="291"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B68" s="377"/>
-      <c r="C68" s="357"/>
-      <c r="D68" s="358"/>
+      <c r="B68" s="395"/>
+      <c r="C68" s="399"/>
+      <c r="D68" s="400"/>
       <c r="E68" s="149"/>
       <c r="F68" s="185"/>
       <c r="G68" s="185"/>
@@ -15370,9 +15368,9 @@
       <c r="J68" s="291"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B69" s="377"/>
-      <c r="C69" s="357"/>
-      <c r="D69" s="358"/>
+      <c r="B69" s="395"/>
+      <c r="C69" s="399"/>
+      <c r="D69" s="400"/>
       <c r="E69" s="149"/>
       <c r="F69" s="185"/>
       <c r="G69" s="185"/>
@@ -15381,9 +15379,9 @@
       <c r="J69" s="291"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B70" s="377"/>
-      <c r="C70" s="357"/>
-      <c r="D70" s="358"/>
+      <c r="B70" s="395"/>
+      <c r="C70" s="399"/>
+      <c r="D70" s="400"/>
       <c r="E70" s="149"/>
       <c r="F70" s="185"/>
       <c r="G70" s="185"/>
@@ -15392,9 +15390,9 @@
       <c r="J70" s="266"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B71" s="377"/>
-      <c r="C71" s="357"/>
-      <c r="D71" s="358"/>
+      <c r="B71" s="395"/>
+      <c r="C71" s="399"/>
+      <c r="D71" s="400"/>
       <c r="E71" s="149"/>
       <c r="F71" s="185"/>
       <c r="G71" s="185"/>
@@ -15403,9 +15401,9 @@
       <c r="J71" s="266"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B72" s="377"/>
-      <c r="C72" s="357"/>
-      <c r="D72" s="358"/>
+      <c r="B72" s="395"/>
+      <c r="C72" s="399"/>
+      <c r="D72" s="400"/>
       <c r="E72" s="149"/>
       <c r="F72" s="185"/>
       <c r="G72" s="185"/>
@@ -15414,9 +15412,9 @@
       <c r="J72" s="266"/>
     </row>
     <row r="73" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="378"/>
-      <c r="C73" s="379"/>
-      <c r="D73" s="380"/>
+      <c r="B73" s="396"/>
+      <c r="C73" s="401"/>
+      <c r="D73" s="402"/>
       <c r="E73" s="149"/>
       <c r="F73" s="185"/>
       <c r="G73" s="185"/>
@@ -15425,11 +15423,11 @@
       <c r="J73" s="266"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B74" s="376" t="s">
+      <c r="B74" s="394" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="355"/>
-      <c r="D74" s="356"/>
+      <c r="C74" s="397"/>
+      <c r="D74" s="398"/>
       <c r="E74" s="149"/>
       <c r="F74" s="185"/>
       <c r="G74" s="185"/>
@@ -15438,9 +15436,9 @@
       <c r="J74" s="266"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B75" s="377"/>
-      <c r="C75" s="357"/>
-      <c r="D75" s="358"/>
+      <c r="B75" s="395"/>
+      <c r="C75" s="399"/>
+      <c r="D75" s="400"/>
       <c r="E75" s="149"/>
       <c r="F75" s="185"/>
       <c r="G75" s="185"/>
@@ -15449,688 +15447,688 @@
       <c r="J75" s="266"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B76" s="377"/>
-      <c r="C76" s="357"/>
-      <c r="D76" s="358"/>
+      <c r="B76" s="395"/>
+      <c r="C76" s="399"/>
+      <c r="D76" s="400"/>
       <c r="E76" s="149"/>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B77" s="377"/>
-      <c r="C77" s="357"/>
-      <c r="D77" s="358"/>
+      <c r="B77" s="395"/>
+      <c r="C77" s="399"/>
+      <c r="D77" s="400"/>
       <c r="E77" s="149"/>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B78" s="377"/>
-      <c r="C78" s="357"/>
-      <c r="D78" s="358"/>
+      <c r="B78" s="395"/>
+      <c r="C78" s="399"/>
+      <c r="D78" s="400"/>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B79" s="377"/>
-      <c r="C79" s="357"/>
-      <c r="D79" s="358"/>
+      <c r="B79" s="395"/>
+      <c r="C79" s="399"/>
+      <c r="D79" s="400"/>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B80" s="377"/>
-      <c r="C80" s="357"/>
-      <c r="D80" s="358"/>
+      <c r="B80" s="395"/>
+      <c r="C80" s="399"/>
+      <c r="D80" s="400"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B81" s="377"/>
-      <c r="C81" s="357"/>
-      <c r="D81" s="358"/>
+      <c r="B81" s="395"/>
+      <c r="C81" s="399"/>
+      <c r="D81" s="400"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B82" s="377"/>
-      <c r="C82" s="357"/>
-      <c r="D82" s="358"/>
+      <c r="B82" s="395"/>
+      <c r="C82" s="399"/>
+      <c r="D82" s="400"/>
     </row>
     <row r="83" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="378"/>
-      <c r="C83" s="379"/>
-      <c r="D83" s="380"/>
+      <c r="B83" s="396"/>
+      <c r="C83" s="401"/>
+      <c r="D83" s="402"/>
     </row>
     <row r="84" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="376" t="s">
+      <c r="B84" s="394" t="s">
         <v>37</v>
       </c>
-      <c r="C84" s="355"/>
-      <c r="D84" s="356"/>
+      <c r="C84" s="397"/>
+      <c r="D84" s="398"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B85" s="377"/>
-      <c r="C85" s="371" t="s">
+      <c r="B85" s="395"/>
+      <c r="C85" s="368" t="s">
         <v>147</v>
       </c>
-      <c r="D85" s="372"/>
+      <c r="D85" s="369"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B86" s="377"/>
-      <c r="C86" s="362" t="s">
+      <c r="B86" s="395"/>
+      <c r="C86" s="376" t="s">
         <v>146</v>
       </c>
-      <c r="D86" s="363"/>
+      <c r="D86" s="373"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B87" s="377"/>
-      <c r="C87" s="362" t="s">
+      <c r="B87" s="395"/>
+      <c r="C87" s="376" t="s">
         <v>148</v>
       </c>
-      <c r="D87" s="363"/>
+      <c r="D87" s="373"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B88" s="377"/>
-      <c r="C88" s="362" t="s">
+      <c r="B88" s="395"/>
+      <c r="C88" s="376" t="s">
         <v>150</v>
       </c>
-      <c r="D88" s="363"/>
+      <c r="D88" s="373"/>
     </row>
     <row r="89" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="377"/>
-      <c r="C89" s="364" t="s">
+      <c r="B89" s="395"/>
+      <c r="C89" s="370" t="s">
         <v>149</v>
       </c>
-      <c r="D89" s="365"/>
+      <c r="D89" s="371"/>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B90" s="377"/>
-      <c r="C90" s="357"/>
-      <c r="D90" s="358"/>
+      <c r="B90" s="395"/>
+      <c r="C90" s="399"/>
+      <c r="D90" s="400"/>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B91" s="377"/>
-      <c r="C91" s="357"/>
-      <c r="D91" s="358"/>
+      <c r="B91" s="395"/>
+      <c r="C91" s="399"/>
+      <c r="D91" s="400"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B92" s="377"/>
-      <c r="C92" s="357"/>
-      <c r="D92" s="358"/>
+      <c r="B92" s="395"/>
+      <c r="C92" s="399"/>
+      <c r="D92" s="400"/>
       <c r="F92" s="149"/>
     </row>
     <row r="93" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="378"/>
-      <c r="C93" s="379"/>
-      <c r="D93" s="380"/>
+      <c r="B93" s="396"/>
+      <c r="C93" s="401"/>
+      <c r="D93" s="402"/>
       <c r="F93" s="149"/>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B94" s="376" t="s">
+      <c r="B94" s="394" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="355"/>
-      <c r="D94" s="356"/>
+      <c r="C94" s="397"/>
+      <c r="D94" s="398"/>
       <c r="F94" s="149"/>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B95" s="377"/>
-      <c r="C95" s="357"/>
-      <c r="D95" s="358"/>
+      <c r="B95" s="395"/>
+      <c r="C95" s="399"/>
+      <c r="D95" s="400"/>
       <c r="F95" s="149"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B96" s="377"/>
-      <c r="C96" s="357"/>
-      <c r="D96" s="358"/>
+      <c r="B96" s="395"/>
+      <c r="C96" s="399"/>
+      <c r="D96" s="400"/>
       <c r="F96" s="149"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="377"/>
-      <c r="C97" s="357"/>
-      <c r="D97" s="358"/>
+      <c r="B97" s="395"/>
+      <c r="C97" s="399"/>
+      <c r="D97" s="400"/>
       <c r="F97" s="149"/>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B98" s="377"/>
-      <c r="C98" s="357"/>
-      <c r="D98" s="358"/>
+      <c r="B98" s="395"/>
+      <c r="C98" s="399"/>
+      <c r="D98" s="400"/>
       <c r="F98" s="149"/>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B99" s="377"/>
-      <c r="C99" s="357"/>
-      <c r="D99" s="358"/>
+      <c r="B99" s="395"/>
+      <c r="C99" s="399"/>
+      <c r="D99" s="400"/>
       <c r="F99" s="149"/>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B100" s="377"/>
-      <c r="C100" s="357"/>
-      <c r="D100" s="358"/>
+      <c r="B100" s="395"/>
+      <c r="C100" s="399"/>
+      <c r="D100" s="400"/>
       <c r="F100" s="149"/>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B101" s="377"/>
-      <c r="C101" s="357"/>
-      <c r="D101" s="358"/>
+      <c r="B101" s="395"/>
+      <c r="C101" s="399"/>
+      <c r="D101" s="400"/>
       <c r="F101" s="149"/>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B102" s="377"/>
-      <c r="C102" s="357"/>
-      <c r="D102" s="358"/>
+      <c r="B102" s="395"/>
+      <c r="C102" s="399"/>
+      <c r="D102" s="400"/>
       <c r="F102" s="149"/>
     </row>
     <row r="103" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="378"/>
-      <c r="C103" s="379"/>
-      <c r="D103" s="380"/>
+      <c r="B103" s="396"/>
+      <c r="C103" s="401"/>
+      <c r="D103" s="402"/>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B104" s="376" t="s">
+      <c r="B104" s="394" t="s">
         <v>16</v>
       </c>
-      <c r="C104" s="355"/>
-      <c r="D104" s="356"/>
+      <c r="C104" s="397"/>
+      <c r="D104" s="398"/>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B105" s="377"/>
-      <c r="C105" s="357" t="s">
+      <c r="B105" s="395"/>
+      <c r="C105" s="399" t="s">
         <v>195</v>
       </c>
-      <c r="D105" s="358"/>
+      <c r="D105" s="400"/>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B106" s="377"/>
-      <c r="C106" s="357"/>
-      <c r="D106" s="358"/>
+      <c r="B106" s="395"/>
+      <c r="C106" s="399"/>
+      <c r="D106" s="400"/>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B107" s="377"/>
-      <c r="C107" s="357"/>
-      <c r="D107" s="358"/>
+      <c r="B107" s="395"/>
+      <c r="C107" s="399"/>
+      <c r="D107" s="400"/>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B108" s="377"/>
-      <c r="C108" s="357"/>
-      <c r="D108" s="358"/>
+      <c r="B108" s="395"/>
+      <c r="C108" s="399"/>
+      <c r="D108" s="400"/>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B109" s="377"/>
-      <c r="C109" s="357"/>
-      <c r="D109" s="358"/>
+      <c r="B109" s="395"/>
+      <c r="C109" s="399"/>
+      <c r="D109" s="400"/>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B110" s="377"/>
-      <c r="C110" s="357"/>
-      <c r="D110" s="358"/>
+      <c r="B110" s="395"/>
+      <c r="C110" s="399"/>
+      <c r="D110" s="400"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B111" s="377"/>
-      <c r="C111" s="357"/>
-      <c r="D111" s="358"/>
+      <c r="B111" s="395"/>
+      <c r="C111" s="399"/>
+      <c r="D111" s="400"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B112" s="377"/>
-      <c r="C112" s="357"/>
-      <c r="D112" s="358"/>
+      <c r="B112" s="395"/>
+      <c r="C112" s="399"/>
+      <c r="D112" s="400"/>
     </row>
     <row r="113" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B113" s="378"/>
-      <c r="C113" s="379"/>
-      <c r="D113" s="380"/>
+      <c r="B113" s="396"/>
+      <c r="C113" s="401"/>
+      <c r="D113" s="402"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B114" s="376" t="s">
+      <c r="B114" s="394" t="s">
         <v>69</v>
       </c>
-      <c r="C114" s="355"/>
-      <c r="D114" s="356"/>
+      <c r="C114" s="397"/>
+      <c r="D114" s="398"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B115" s="377"/>
-      <c r="C115" s="357"/>
-      <c r="D115" s="358"/>
+      <c r="B115" s="395"/>
+      <c r="C115" s="399"/>
+      <c r="D115" s="400"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B116" s="377"/>
-      <c r="C116" s="357"/>
-      <c r="D116" s="358"/>
+      <c r="B116" s="395"/>
+      <c r="C116" s="399"/>
+      <c r="D116" s="400"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B117" s="377"/>
-      <c r="C117" s="357"/>
-      <c r="D117" s="358"/>
+      <c r="B117" s="395"/>
+      <c r="C117" s="399"/>
+      <c r="D117" s="400"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B118" s="377"/>
-      <c r="C118" s="357"/>
-      <c r="D118" s="358"/>
+      <c r="B118" s="395"/>
+      <c r="C118" s="399"/>
+      <c r="D118" s="400"/>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B119" s="377"/>
-      <c r="C119" s="357"/>
-      <c r="D119" s="358"/>
+      <c r="B119" s="395"/>
+      <c r="C119" s="399"/>
+      <c r="D119" s="400"/>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B120" s="377"/>
-      <c r="C120" s="357"/>
-      <c r="D120" s="358"/>
+      <c r="B120" s="395"/>
+      <c r="C120" s="399"/>
+      <c r="D120" s="400"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B121" s="377"/>
-      <c r="C121" s="357"/>
-      <c r="D121" s="358"/>
+      <c r="B121" s="395"/>
+      <c r="C121" s="399"/>
+      <c r="D121" s="400"/>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B122" s="377"/>
-      <c r="C122" s="357"/>
-      <c r="D122" s="358"/>
+      <c r="B122" s="395"/>
+      <c r="C122" s="399"/>
+      <c r="D122" s="400"/>
     </row>
     <row r="123" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B123" s="378"/>
-      <c r="C123" s="379"/>
-      <c r="D123" s="380"/>
+      <c r="B123" s="396"/>
+      <c r="C123" s="401"/>
+      <c r="D123" s="402"/>
     </row>
     <row r="132" spans="6:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="133" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F133" s="395" t="s">
+      <c r="F133" s="352" t="s">
         <v>68</v>
       </c>
-      <c r="G133" s="395" t="s">
+      <c r="G133" s="352" t="s">
         <v>88</v>
       </c>
       <c r="H133" s="256"/>
       <c r="I133" s="256"/>
-      <c r="J133" s="408"/>
+      <c r="J133" s="387"/>
     </row>
     <row r="134" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F134" s="396"/>
-      <c r="G134" s="392"/>
+      <c r="F134" s="353"/>
+      <c r="G134" s="379"/>
       <c r="H134" s="260"/>
       <c r="I134" s="260"/>
-      <c r="J134" s="400"/>
+      <c r="J134" s="388"/>
     </row>
     <row r="135" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F135" s="396"/>
-      <c r="G135" s="391" t="s">
+      <c r="F135" s="353"/>
+      <c r="G135" s="378" t="s">
         <v>112</v>
       </c>
       <c r="H135" s="257"/>
       <c r="I135" s="257"/>
-      <c r="J135" s="406"/>
+      <c r="J135" s="385"/>
     </row>
     <row r="136" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F136" s="396"/>
-      <c r="G136" s="392"/>
+      <c r="F136" s="353"/>
+      <c r="G136" s="379"/>
       <c r="H136" s="258"/>
       <c r="I136" s="258"/>
-      <c r="J136" s="407"/>
+      <c r="J136" s="386"/>
     </row>
     <row r="137" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F137" s="396"/>
-      <c r="G137" s="391" t="s">
+      <c r="F137" s="353"/>
+      <c r="G137" s="378" t="s">
         <v>79</v>
       </c>
       <c r="H137" s="257"/>
       <c r="I137" s="257"/>
-      <c r="J137" s="406"/>
+      <c r="J137" s="385"/>
     </row>
     <row r="138" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F138" s="396"/>
-      <c r="G138" s="392"/>
+      <c r="F138" s="353"/>
+      <c r="G138" s="379"/>
       <c r="H138" s="258"/>
       <c r="I138" s="258"/>
-      <c r="J138" s="407"/>
+      <c r="J138" s="386"/>
     </row>
     <row r="139" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F139" s="396"/>
-      <c r="G139" s="391" t="s">
+      <c r="F139" s="353"/>
+      <c r="G139" s="378" t="s">
         <v>89</v>
       </c>
       <c r="H139" s="259"/>
       <c r="I139" s="259"/>
-      <c r="J139" s="393"/>
+      <c r="J139" s="362"/>
     </row>
     <row r="140" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F140" s="396"/>
-      <c r="G140" s="392"/>
+      <c r="F140" s="353"/>
+      <c r="G140" s="379"/>
       <c r="H140" s="260"/>
       <c r="I140" s="260"/>
-      <c r="J140" s="393"/>
+      <c r="J140" s="362"/>
     </row>
     <row r="141" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F141" s="396"/>
-      <c r="G141" s="391" t="s">
+      <c r="F141" s="353"/>
+      <c r="G141" s="378" t="s">
         <v>67</v>
       </c>
       <c r="H141" s="259"/>
       <c r="I141" s="259"/>
-      <c r="J141" s="400"/>
+      <c r="J141" s="388"/>
     </row>
     <row r="142" spans="6:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F142" s="394"/>
-      <c r="G142" s="394"/>
+      <c r="F142" s="354"/>
+      <c r="G142" s="354"/>
       <c r="H142" s="276"/>
       <c r="I142" s="276"/>
-      <c r="J142" s="403"/>
+      <c r="J142" s="391"/>
     </row>
     <row r="143" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F143" s="395" t="s">
+      <c r="F143" s="352" t="s">
         <v>37</v>
       </c>
-      <c r="G143" s="395" t="s">
+      <c r="G143" s="352" t="s">
         <v>88</v>
       </c>
       <c r="H143" s="256"/>
       <c r="I143" s="256"/>
-      <c r="J143" s="397"/>
+      <c r="J143" s="403"/>
     </row>
     <row r="144" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F144" s="396"/>
-      <c r="G144" s="392"/>
+      <c r="F144" s="353"/>
+      <c r="G144" s="379"/>
       <c r="H144" s="260"/>
       <c r="I144" s="260"/>
-      <c r="J144" s="398"/>
+      <c r="J144" s="381"/>
     </row>
     <row r="145" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F145" s="396"/>
-      <c r="G145" s="391" t="s">
+      <c r="F145" s="353"/>
+      <c r="G145" s="378" t="s">
         <v>112</v>
       </c>
       <c r="H145" s="259"/>
       <c r="I145" s="259"/>
-      <c r="J145" s="399"/>
+      <c r="J145" s="380"/>
     </row>
     <row r="146" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F146" s="396"/>
-      <c r="G146" s="392"/>
+      <c r="F146" s="353"/>
+      <c r="G146" s="379"/>
       <c r="H146" s="260"/>
       <c r="I146" s="260"/>
-      <c r="J146" s="398"/>
+      <c r="J146" s="381"/>
     </row>
     <row r="147" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F147" s="396"/>
-      <c r="G147" s="391" t="s">
+      <c r="F147" s="353"/>
+      <c r="G147" s="378" t="s">
         <v>79</v>
       </c>
       <c r="H147" s="259"/>
       <c r="I147" s="259"/>
-      <c r="J147" s="400"/>
+      <c r="J147" s="388"/>
     </row>
     <row r="148" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F148" s="396"/>
-      <c r="G148" s="392"/>
+      <c r="F148" s="353"/>
+      <c r="G148" s="379"/>
       <c r="H148" s="260"/>
       <c r="I148" s="260"/>
-      <c r="J148" s="400"/>
+      <c r="J148" s="388"/>
     </row>
     <row r="149" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F149" s="396"/>
-      <c r="G149" s="391" t="s">
+      <c r="F149" s="353"/>
+      <c r="G149" s="378" t="s">
         <v>89</v>
       </c>
       <c r="H149" s="259"/>
       <c r="I149" s="259"/>
-      <c r="J149" s="393"/>
+      <c r="J149" s="362"/>
     </row>
     <row r="150" spans="6:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F150" s="396"/>
-      <c r="G150" s="392"/>
+      <c r="F150" s="353"/>
+      <c r="G150" s="379"/>
       <c r="H150" s="275"/>
       <c r="I150" s="275"/>
-      <c r="J150" s="404"/>
+      <c r="J150" s="363"/>
     </row>
     <row r="151" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F151" s="396"/>
-      <c r="G151" s="391" t="s">
+      <c r="F151" s="353"/>
+      <c r="G151" s="378" t="s">
         <v>67</v>
       </c>
       <c r="H151" s="259"/>
       <c r="I151" s="259"/>
-      <c r="J151" s="400"/>
+      <c r="J151" s="388"/>
     </row>
     <row r="152" spans="6:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F152" s="394"/>
-      <c r="G152" s="394"/>
+      <c r="F152" s="354"/>
+      <c r="G152" s="354"/>
       <c r="H152" s="276"/>
       <c r="I152" s="276"/>
-      <c r="J152" s="403"/>
+      <c r="J152" s="391"/>
     </row>
     <row r="153" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F153" s="395" t="s">
+      <c r="F153" s="352" t="s">
         <v>8</v>
       </c>
-      <c r="G153" s="395" t="s">
+      <c r="G153" s="352" t="s">
         <v>88</v>
       </c>
       <c r="H153" s="256"/>
       <c r="I153" s="256"/>
-      <c r="J153" s="397"/>
+      <c r="J153" s="403"/>
     </row>
     <row r="154" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F154" s="396"/>
-      <c r="G154" s="392"/>
+      <c r="F154" s="353"/>
+      <c r="G154" s="379"/>
       <c r="H154" s="260"/>
       <c r="I154" s="260"/>
-      <c r="J154" s="398"/>
+      <c r="J154" s="381"/>
     </row>
     <row r="155" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F155" s="396"/>
-      <c r="G155" s="391" t="s">
+      <c r="F155" s="353"/>
+      <c r="G155" s="378" t="s">
         <v>112</v>
       </c>
       <c r="H155" s="259"/>
       <c r="I155" s="259"/>
-      <c r="J155" s="399"/>
+      <c r="J155" s="380"/>
     </row>
     <row r="156" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F156" s="396"/>
-      <c r="G156" s="392"/>
+      <c r="F156" s="353"/>
+      <c r="G156" s="379"/>
       <c r="H156" s="260"/>
       <c r="I156" s="260"/>
-      <c r="J156" s="398"/>
+      <c r="J156" s="381"/>
     </row>
     <row r="157" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F157" s="396"/>
-      <c r="G157" s="391" t="s">
+      <c r="F157" s="353"/>
+      <c r="G157" s="378" t="s">
         <v>79</v>
       </c>
       <c r="H157" s="259"/>
       <c r="I157" s="259"/>
-      <c r="J157" s="400"/>
+      <c r="J157" s="388"/>
     </row>
     <row r="158" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F158" s="396"/>
-      <c r="G158" s="392"/>
+      <c r="F158" s="353"/>
+      <c r="G158" s="379"/>
       <c r="H158" s="260"/>
       <c r="I158" s="260"/>
-      <c r="J158" s="400"/>
+      <c r="J158" s="388"/>
     </row>
     <row r="159" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F159" s="396"/>
-      <c r="G159" s="391" t="s">
+      <c r="F159" s="353"/>
+      <c r="G159" s="378" t="s">
         <v>89</v>
       </c>
       <c r="H159" s="259"/>
       <c r="I159" s="259"/>
-      <c r="J159" s="393"/>
+      <c r="J159" s="362"/>
     </row>
     <row r="160" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F160" s="396"/>
-      <c r="G160" s="392"/>
+      <c r="F160" s="353"/>
+      <c r="G160" s="379"/>
       <c r="H160" s="260"/>
       <c r="I160" s="260"/>
-      <c r="J160" s="393"/>
+      <c r="J160" s="362"/>
     </row>
     <row r="161" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F161" s="396"/>
-      <c r="G161" s="391" t="s">
+      <c r="F161" s="353"/>
+      <c r="G161" s="378" t="s">
         <v>67</v>
       </c>
       <c r="H161" s="259"/>
       <c r="I161" s="259"/>
-      <c r="J161" s="400"/>
+      <c r="J161" s="388"/>
     </row>
     <row r="162" spans="6:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F162" s="394"/>
-      <c r="G162" s="394"/>
+      <c r="F162" s="354"/>
+      <c r="G162" s="354"/>
       <c r="H162" s="276"/>
       <c r="I162" s="276"/>
-      <c r="J162" s="403"/>
+      <c r="J162" s="391"/>
     </row>
     <row r="163" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F163" s="395" t="s">
+      <c r="F163" s="352" t="s">
         <v>16</v>
       </c>
-      <c r="G163" s="395" t="s">
+      <c r="G163" s="352" t="s">
         <v>88</v>
       </c>
       <c r="H163" s="256"/>
       <c r="I163" s="256"/>
-      <c r="J163" s="397"/>
+      <c r="J163" s="403"/>
     </row>
     <row r="164" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F164" s="396"/>
-      <c r="G164" s="392"/>
+      <c r="F164" s="353"/>
+      <c r="G164" s="379"/>
       <c r="H164" s="260"/>
       <c r="I164" s="260"/>
-      <c r="J164" s="398"/>
+      <c r="J164" s="381"/>
     </row>
     <row r="165" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F165" s="396"/>
-      <c r="G165" s="391" t="s">
+      <c r="F165" s="353"/>
+      <c r="G165" s="378" t="s">
         <v>112</v>
       </c>
       <c r="H165" s="259"/>
       <c r="I165" s="259"/>
-      <c r="J165" s="399"/>
+      <c r="J165" s="380"/>
     </row>
     <row r="166" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F166" s="396"/>
-      <c r="G166" s="392"/>
+      <c r="F166" s="353"/>
+      <c r="G166" s="379"/>
       <c r="H166" s="260"/>
       <c r="I166" s="260"/>
-      <c r="J166" s="398"/>
+      <c r="J166" s="381"/>
     </row>
     <row r="167" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F167" s="396"/>
-      <c r="G167" s="391" t="s">
+      <c r="F167" s="353"/>
+      <c r="G167" s="378" t="s">
         <v>79</v>
       </c>
       <c r="H167" s="259"/>
       <c r="I167" s="259"/>
-      <c r="J167" s="400"/>
+      <c r="J167" s="388"/>
     </row>
     <row r="168" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F168" s="396"/>
-      <c r="G168" s="392"/>
+      <c r="F168" s="353"/>
+      <c r="G168" s="379"/>
       <c r="H168" s="260"/>
       <c r="I168" s="260"/>
-      <c r="J168" s="400"/>
+      <c r="J168" s="388"/>
     </row>
     <row r="169" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F169" s="396"/>
-      <c r="G169" s="391" t="s">
+      <c r="F169" s="353"/>
+      <c r="G169" s="378" t="s">
         <v>89</v>
       </c>
       <c r="H169" s="259"/>
       <c r="I169" s="259"/>
-      <c r="J169" s="393"/>
+      <c r="J169" s="362"/>
     </row>
     <row r="170" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F170" s="396"/>
-      <c r="G170" s="392"/>
+      <c r="F170" s="353"/>
+      <c r="G170" s="379"/>
       <c r="H170" s="260"/>
       <c r="I170" s="260"/>
-      <c r="J170" s="393"/>
+      <c r="J170" s="362"/>
     </row>
     <row r="171" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F171" s="396"/>
-      <c r="G171" s="391" t="s">
+      <c r="F171" s="353"/>
+      <c r="G171" s="378" t="s">
         <v>67</v>
       </c>
       <c r="H171" s="259"/>
       <c r="I171" s="259"/>
-      <c r="J171" s="400"/>
+      <c r="J171" s="388"/>
     </row>
     <row r="172" spans="6:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F172" s="394"/>
-      <c r="G172" s="394"/>
+      <c r="F172" s="354"/>
+      <c r="G172" s="354"/>
       <c r="H172" s="276"/>
       <c r="I172" s="276"/>
-      <c r="J172" s="403"/>
+      <c r="J172" s="391"/>
     </row>
     <row r="173" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F173" s="395" t="s">
+      <c r="F173" s="352" t="s">
         <v>167</v>
       </c>
-      <c r="G173" s="395" t="s">
+      <c r="G173" s="352" t="s">
         <v>88</v>
       </c>
       <c r="H173" s="256"/>
       <c r="I173" s="256"/>
-      <c r="J173" s="397"/>
+      <c r="J173" s="403"/>
     </row>
     <row r="174" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F174" s="396"/>
-      <c r="G174" s="392"/>
+      <c r="F174" s="353"/>
+      <c r="G174" s="379"/>
       <c r="H174" s="260"/>
       <c r="I174" s="260"/>
-      <c r="J174" s="398"/>
+      <c r="J174" s="381"/>
     </row>
     <row r="175" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F175" s="396"/>
-      <c r="G175" s="391" t="s">
+      <c r="F175" s="353"/>
+      <c r="G175" s="378" t="s">
         <v>112</v>
       </c>
       <c r="H175" s="259"/>
       <c r="I175" s="259"/>
-      <c r="J175" s="399"/>
+      <c r="J175" s="380"/>
     </row>
     <row r="176" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F176" s="396"/>
-      <c r="G176" s="392"/>
+      <c r="F176" s="353"/>
+      <c r="G176" s="379"/>
       <c r="H176" s="260"/>
       <c r="I176" s="260"/>
-      <c r="J176" s="398"/>
+      <c r="J176" s="381"/>
     </row>
     <row r="177" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F177" s="396"/>
-      <c r="G177" s="391" t="s">
+      <c r="F177" s="353"/>
+      <c r="G177" s="378" t="s">
         <v>79</v>
       </c>
       <c r="H177" s="259"/>
       <c r="I177" s="259"/>
-      <c r="J177" s="400"/>
+      <c r="J177" s="388"/>
     </row>
     <row r="178" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F178" s="396"/>
-      <c r="G178" s="392"/>
+      <c r="F178" s="353"/>
+      <c r="G178" s="379"/>
       <c r="H178" s="260"/>
       <c r="I178" s="260"/>
-      <c r="J178" s="400"/>
+      <c r="J178" s="388"/>
     </row>
     <row r="179" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F179" s="396"/>
-      <c r="G179" s="391" t="s">
+      <c r="F179" s="353"/>
+      <c r="G179" s="378" t="s">
         <v>89</v>
       </c>
       <c r="H179" s="259"/>
       <c r="I179" s="259"/>
-      <c r="J179" s="393"/>
+      <c r="J179" s="362"/>
     </row>
     <row r="180" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F180" s="396"/>
-      <c r="G180" s="392"/>
+      <c r="F180" s="353"/>
+      <c r="G180" s="379"/>
       <c r="H180" s="260"/>
       <c r="I180" s="260"/>
-      <c r="J180" s="393"/>
+      <c r="J180" s="362"/>
     </row>
     <row r="181" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F181" s="396"/>
-      <c r="G181" s="391" t="s">
+      <c r="F181" s="353"/>
+      <c r="G181" s="378" t="s">
         <v>67</v>
       </c>
       <c r="H181" s="259"/>
       <c r="I181" s="259"/>
-      <c r="J181" s="401"/>
+      <c r="J181" s="365"/>
     </row>
     <row r="182" spans="6:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F182" s="394"/>
-      <c r="G182" s="394"/>
+      <c r="F182" s="354"/>
+      <c r="G182" s="354"/>
       <c r="H182" s="276"/>
       <c r="I182" s="276"/>
-      <c r="J182" s="402"/>
+      <c r="J182" s="366"/>
     </row>
     <row r="199" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="200" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -16193,13 +16191,13 @@
       <c r="E214" s="281"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A215" s="395" t="s">
+      <c r="A215" s="352" t="s">
         <v>200</v>
       </c>
-      <c r="B215" s="417" t="s">
+      <c r="B215" s="355" t="s">
         <v>88</v>
       </c>
-      <c r="C215" s="411" t="s">
+      <c r="C215" s="358" t="s">
         <v>170</v>
       </c>
       <c r="D215" s="283">
@@ -16208,195 +16206,195 @@
       <c r="E215" s="282"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A216" s="396"/>
-      <c r="B216" s="418"/>
-      <c r="C216" s="412"/>
+      <c r="A216" s="353"/>
+      <c r="B216" s="356"/>
+      <c r="C216" s="359"/>
       <c r="D216" s="284">
         <v>2</v>
       </c>
       <c r="E216" s="280"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A217" s="396"/>
-      <c r="B217" s="418"/>
-      <c r="C217" s="412"/>
+      <c r="A217" s="353"/>
+      <c r="B217" s="356"/>
+      <c r="C217" s="359"/>
       <c r="D217" s="284">
         <v>3</v>
       </c>
       <c r="E217" s="280"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A218" s="396"/>
-      <c r="B218" s="418"/>
-      <c r="C218" s="412"/>
+      <c r="A218" s="353"/>
+      <c r="B218" s="356"/>
+      <c r="C218" s="359"/>
       <c r="D218" s="284">
         <v>4</v>
       </c>
       <c r="E218" s="280"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A219" s="396"/>
-      <c r="B219" s="418"/>
-      <c r="C219" s="412"/>
+      <c r="A219" s="353"/>
+      <c r="B219" s="356"/>
+      <c r="C219" s="359"/>
       <c r="D219" s="284">
         <v>5</v>
       </c>
       <c r="E219" s="280"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A220" s="396"/>
-      <c r="B220" s="418"/>
-      <c r="C220" s="412"/>
+      <c r="A220" s="353"/>
+      <c r="B220" s="356"/>
+      <c r="C220" s="359"/>
       <c r="D220" s="284">
         <v>6</v>
       </c>
       <c r="E220" s="280"/>
     </row>
     <row r="221" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A221" s="396"/>
-      <c r="B221" s="419"/>
-      <c r="C221" s="413"/>
+      <c r="A221" s="353"/>
+      <c r="B221" s="357"/>
+      <c r="C221" s="360"/>
       <c r="D221" s="285">
         <v>7</v>
       </c>
       <c r="E221" s="281"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A222" s="396"/>
-      <c r="B222" s="417" t="s">
+      <c r="A222" s="353"/>
+      <c r="B222" s="355" t="s">
         <v>112</v>
       </c>
-      <c r="C222" s="411"/>
+      <c r="C222" s="358"/>
       <c r="D222" s="283">
         <v>8</v>
       </c>
       <c r="E222" s="282"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223" s="396"/>
-      <c r="B223" s="418"/>
-      <c r="C223" s="412"/>
+      <c r="A223" s="353"/>
+      <c r="B223" s="356"/>
+      <c r="C223" s="359"/>
       <c r="D223" s="284">
         <v>9</v>
       </c>
       <c r="E223" s="280"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A224" s="396"/>
-      <c r="B224" s="418"/>
-      <c r="C224" s="412"/>
+      <c r="A224" s="353"/>
+      <c r="B224" s="356"/>
+      <c r="C224" s="359"/>
       <c r="D224" s="284">
         <v>10</v>
       </c>
       <c r="E224" s="280"/>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A225" s="396"/>
-      <c r="B225" s="418"/>
-      <c r="C225" s="412"/>
+      <c r="A225" s="353"/>
+      <c r="B225" s="356"/>
+      <c r="C225" s="359"/>
       <c r="D225" s="284">
         <v>11</v>
       </c>
       <c r="E225" s="280"/>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A226" s="396"/>
-      <c r="B226" s="418"/>
-      <c r="C226" s="412"/>
+      <c r="A226" s="353"/>
+      <c r="B226" s="356"/>
+      <c r="C226" s="359"/>
       <c r="D226" s="284">
         <v>12</v>
       </c>
       <c r="E226" s="280"/>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A227" s="396"/>
-      <c r="B227" s="418"/>
-      <c r="C227" s="412"/>
+      <c r="A227" s="353"/>
+      <c r="B227" s="356"/>
+      <c r="C227" s="359"/>
       <c r="D227" s="284">
         <v>13</v>
       </c>
       <c r="E227" s="280"/>
     </row>
     <row r="228" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A228" s="396"/>
-      <c r="B228" s="419"/>
-      <c r="C228" s="413"/>
+      <c r="A228" s="353"/>
+      <c r="B228" s="357"/>
+      <c r="C228" s="360"/>
       <c r="D228" s="285">
         <v>14</v>
       </c>
       <c r="E228" s="281"/>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A229" s="396"/>
-      <c r="B229" s="417" t="s">
+      <c r="A229" s="353"/>
+      <c r="B229" s="355" t="s">
         <v>79</v>
       </c>
-      <c r="C229" s="411"/>
+      <c r="C229" s="358"/>
       <c r="D229" s="283">
         <v>15</v>
       </c>
       <c r="E229" s="282"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A230" s="396"/>
-      <c r="B230" s="418"/>
-      <c r="C230" s="412"/>
+      <c r="A230" s="353"/>
+      <c r="B230" s="356"/>
+      <c r="C230" s="359"/>
       <c r="D230" s="284">
         <v>16</v>
       </c>
       <c r="E230" s="278"/>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A231" s="396"/>
-      <c r="B231" s="418"/>
-      <c r="C231" s="412"/>
+      <c r="A231" s="353"/>
+      <c r="B231" s="356"/>
+      <c r="C231" s="359"/>
       <c r="D231" s="284">
         <v>17</v>
       </c>
       <c r="E231" s="278"/>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A232" s="396"/>
-      <c r="B232" s="418"/>
-      <c r="C232" s="412"/>
+      <c r="A232" s="353"/>
+      <c r="B232" s="356"/>
+      <c r="C232" s="359"/>
       <c r="D232" s="284">
         <v>18</v>
       </c>
       <c r="E232" s="278"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A233" s="396"/>
-      <c r="B233" s="418"/>
-      <c r="C233" s="412"/>
+      <c r="A233" s="353"/>
+      <c r="B233" s="356"/>
+      <c r="C233" s="359"/>
       <c r="D233" s="284">
         <v>19</v>
       </c>
       <c r="E233" s="278"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A234" s="396"/>
-      <c r="B234" s="418"/>
-      <c r="C234" s="412"/>
+      <c r="A234" s="353"/>
+      <c r="B234" s="356"/>
+      <c r="C234" s="359"/>
       <c r="D234" s="284">
         <v>20</v>
       </c>
       <c r="E234" s="278"/>
     </row>
     <row r="235" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A235" s="396"/>
-      <c r="B235" s="419"/>
-      <c r="C235" s="413"/>
+      <c r="A235" s="353"/>
+      <c r="B235" s="357"/>
+      <c r="C235" s="360"/>
       <c r="D235" s="285">
         <v>21</v>
       </c>
       <c r="E235" s="279"/>
     </row>
     <row r="236" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A236" s="396"/>
-      <c r="B236" s="417" t="s">
+      <c r="A236" s="353"/>
+      <c r="B236" s="355" t="s">
         <v>89</v>
       </c>
-      <c r="C236" s="411"/>
+      <c r="C236" s="358"/>
       <c r="D236" s="283">
         <v>22</v>
       </c>
@@ -16405,113 +16403,113 @@
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A237" s="396"/>
-      <c r="B237" s="418"/>
-      <c r="C237" s="412"/>
+      <c r="A237" s="353"/>
+      <c r="B237" s="356"/>
+      <c r="C237" s="359"/>
       <c r="D237" s="284">
         <v>23</v>
       </c>
       <c r="E237" s="277"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238" s="396"/>
-      <c r="B238" s="418"/>
-      <c r="C238" s="412"/>
+      <c r="A238" s="353"/>
+      <c r="B238" s="356"/>
+      <c r="C238" s="359"/>
       <c r="D238" s="284">
         <v>24</v>
       </c>
       <c r="E238" s="278"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239" s="396"/>
-      <c r="B239" s="418"/>
-      <c r="C239" s="412"/>
+      <c r="A239" s="353"/>
+      <c r="B239" s="356"/>
+      <c r="C239" s="359"/>
       <c r="D239" s="284">
         <v>25</v>
       </c>
       <c r="E239" s="278"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A240" s="396"/>
-      <c r="B240" s="418"/>
-      <c r="C240" s="412"/>
+      <c r="A240" s="353"/>
+      <c r="B240" s="356"/>
+      <c r="C240" s="359"/>
       <c r="D240" s="284">
         <v>26</v>
       </c>
       <c r="E240" s="278"/>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A241" s="396"/>
-      <c r="B241" s="418"/>
-      <c r="C241" s="412"/>
+      <c r="A241" s="353"/>
+      <c r="B241" s="356"/>
+      <c r="C241" s="359"/>
       <c r="D241" s="284">
         <v>27</v>
       </c>
       <c r="E241" s="278"/>
     </row>
     <row r="242" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A242" s="396"/>
-      <c r="B242" s="419"/>
-      <c r="C242" s="413"/>
+      <c r="A242" s="353"/>
+      <c r="B242" s="357"/>
+      <c r="C242" s="360"/>
       <c r="D242" s="285">
         <v>28</v>
       </c>
       <c r="E242" s="278"/>
     </row>
     <row r="243" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A243" s="396"/>
-      <c r="B243" s="417" t="s">
+      <c r="A243" s="353"/>
+      <c r="B243" s="355" t="s">
         <v>67</v>
       </c>
-      <c r="C243" s="411"/>
+      <c r="C243" s="358"/>
       <c r="D243" s="283">
         <v>29</v>
       </c>
       <c r="E243" s="279"/>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A244" s="396"/>
-      <c r="B244" s="418"/>
-      <c r="C244" s="412"/>
+      <c r="A244" s="353"/>
+      <c r="B244" s="356"/>
+      <c r="C244" s="359"/>
       <c r="D244" s="284">
         <v>30</v>
       </c>
       <c r="E244" s="277"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A245" s="396"/>
-      <c r="B245" s="418"/>
-      <c r="C245" s="412"/>
+      <c r="A245" s="353"/>
+      <c r="B245" s="356"/>
+      <c r="C245" s="359"/>
       <c r="D245" s="284">
         <v>31</v>
       </c>
       <c r="E245" s="278"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A246" s="396"/>
-      <c r="B246" s="418"/>
-      <c r="C246" s="412"/>
+      <c r="A246" s="353"/>
+      <c r="B246" s="356"/>
+      <c r="C246" s="359"/>
       <c r="D246" s="286"/>
       <c r="E246" s="278"/>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A247" s="396"/>
-      <c r="B247" s="418"/>
-      <c r="C247" s="412"/>
+      <c r="A247" s="353"/>
+      <c r="B247" s="356"/>
+      <c r="C247" s="359"/>
       <c r="D247" s="286"/>
       <c r="E247" s="278"/>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A248" s="396"/>
-      <c r="B248" s="418"/>
-      <c r="C248" s="412"/>
+      <c r="A248" s="353"/>
+      <c r="B248" s="356"/>
+      <c r="C248" s="359"/>
       <c r="D248" s="286"/>
       <c r="E248" s="278"/>
     </row>
     <row r="249" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A249" s="394"/>
-      <c r="B249" s="419"/>
-      <c r="C249" s="413"/>
+      <c r="A249" s="354"/>
+      <c r="B249" s="357"/>
+      <c r="C249" s="360"/>
       <c r="D249" s="287"/>
       <c r="E249" s="280"/>
     </row>
@@ -16531,13 +16529,13 @@
       <c r="E250" s="281"/>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A251" s="395" t="s">
+      <c r="A251" s="352" t="s">
         <v>200</v>
       </c>
-      <c r="B251" s="417" t="s">
+      <c r="B251" s="355" t="s">
         <v>88</v>
       </c>
-      <c r="C251" s="411" t="s">
+      <c r="C251" s="358" t="s">
         <v>170</v>
       </c>
       <c r="D251" s="283">
@@ -16546,335 +16544,437 @@
       <c r="E251" s="282"/>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A252" s="396"/>
-      <c r="B252" s="418"/>
-      <c r="C252" s="412"/>
+      <c r="A252" s="353"/>
+      <c r="B252" s="356"/>
+      <c r="C252" s="359"/>
       <c r="D252" s="284">
         <v>2</v>
       </c>
       <c r="E252" s="280"/>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A253" s="396"/>
-      <c r="B253" s="418"/>
-      <c r="C253" s="412"/>
+      <c r="A253" s="353"/>
+      <c r="B253" s="356"/>
+      <c r="C253" s="359"/>
       <c r="D253" s="284">
         <v>3</v>
       </c>
       <c r="E253" s="280"/>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A254" s="396"/>
-      <c r="B254" s="418"/>
-      <c r="C254" s="412"/>
+      <c r="A254" s="353"/>
+      <c r="B254" s="356"/>
+      <c r="C254" s="359"/>
       <c r="D254" s="284">
         <v>4</v>
       </c>
       <c r="E254" s="280"/>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A255" s="396"/>
-      <c r="B255" s="418"/>
-      <c r="C255" s="412"/>
+      <c r="A255" s="353"/>
+      <c r="B255" s="356"/>
+      <c r="C255" s="359"/>
       <c r="D255" s="284">
         <v>5</v>
       </c>
       <c r="E255" s="280"/>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A256" s="396"/>
-      <c r="B256" s="418"/>
-      <c r="C256" s="412"/>
+      <c r="A256" s="353"/>
+      <c r="B256" s="356"/>
+      <c r="C256" s="359"/>
       <c r="D256" s="284">
         <v>6</v>
       </c>
       <c r="E256" s="280"/>
     </row>
     <row r="257" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A257" s="396"/>
-      <c r="B257" s="419"/>
-      <c r="C257" s="413"/>
+      <c r="A257" s="353"/>
+      <c r="B257" s="357"/>
+      <c r="C257" s="360"/>
       <c r="D257" s="285">
         <v>7</v>
       </c>
       <c r="E257" s="281"/>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A258" s="396"/>
-      <c r="B258" s="417" t="s">
+      <c r="A258" s="353"/>
+      <c r="B258" s="355" t="s">
         <v>112</v>
       </c>
-      <c r="C258" s="411"/>
+      <c r="C258" s="358"/>
       <c r="D258" s="283">
         <v>8</v>
       </c>
       <c r="E258" s="282"/>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A259" s="396"/>
-      <c r="B259" s="418"/>
-      <c r="C259" s="412"/>
+      <c r="A259" s="353"/>
+      <c r="B259" s="356"/>
+      <c r="C259" s="359"/>
       <c r="D259" s="284">
         <v>9</v>
       </c>
       <c r="E259" s="280"/>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A260" s="396"/>
-      <c r="B260" s="418"/>
-      <c r="C260" s="412"/>
+      <c r="A260" s="353"/>
+      <c r="B260" s="356"/>
+      <c r="C260" s="359"/>
       <c r="D260" s="284">
         <v>10</v>
       </c>
       <c r="E260" s="280"/>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A261" s="396"/>
-      <c r="B261" s="418"/>
-      <c r="C261" s="412"/>
+      <c r="A261" s="353"/>
+      <c r="B261" s="356"/>
+      <c r="C261" s="359"/>
       <c r="D261" s="284">
         <v>11</v>
       </c>
       <c r="E261" s="280"/>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A262" s="396"/>
-      <c r="B262" s="418"/>
-      <c r="C262" s="412"/>
+      <c r="A262" s="353"/>
+      <c r="B262" s="356"/>
+      <c r="C262" s="359"/>
       <c r="D262" s="284">
         <v>12</v>
       </c>
       <c r="E262" s="280"/>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A263" s="396"/>
-      <c r="B263" s="418"/>
-      <c r="C263" s="412"/>
+      <c r="A263" s="353"/>
+      <c r="B263" s="356"/>
+      <c r="C263" s="359"/>
       <c r="D263" s="284">
         <v>13</v>
       </c>
       <c r="E263" s="280"/>
     </row>
     <row r="264" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A264" s="396"/>
-      <c r="B264" s="419"/>
-      <c r="C264" s="413"/>
+      <c r="A264" s="353"/>
+      <c r="B264" s="357"/>
+      <c r="C264" s="360"/>
       <c r="D264" s="285">
         <v>14</v>
       </c>
       <c r="E264" s="281"/>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A265" s="396"/>
-      <c r="B265" s="417" t="s">
+      <c r="A265" s="353"/>
+      <c r="B265" s="355" t="s">
         <v>79</v>
       </c>
-      <c r="C265" s="411"/>
+      <c r="C265" s="358"/>
       <c r="D265" s="283">
         <v>15</v>
       </c>
       <c r="E265" s="282"/>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A266" s="396"/>
-      <c r="B266" s="418"/>
-      <c r="C266" s="412"/>
+      <c r="A266" s="353"/>
+      <c r="B266" s="356"/>
+      <c r="C266" s="359"/>
       <c r="D266" s="284">
         <v>16</v>
       </c>
       <c r="E266" s="278"/>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A267" s="396"/>
-      <c r="B267" s="418"/>
-      <c r="C267" s="412"/>
+      <c r="A267" s="353"/>
+      <c r="B267" s="356"/>
+      <c r="C267" s="359"/>
       <c r="D267" s="284">
         <v>17</v>
       </c>
       <c r="E267" s="278"/>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A268" s="396"/>
-      <c r="B268" s="418"/>
-      <c r="C268" s="412"/>
+      <c r="A268" s="353"/>
+      <c r="B268" s="356"/>
+      <c r="C268" s="359"/>
       <c r="D268" s="284">
         <v>18</v>
       </c>
       <c r="E268" s="278"/>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A269" s="396"/>
-      <c r="B269" s="418"/>
-      <c r="C269" s="412"/>
+      <c r="A269" s="353"/>
+      <c r="B269" s="356"/>
+      <c r="C269" s="359"/>
       <c r="D269" s="284">
         <v>19</v>
       </c>
       <c r="E269" s="278"/>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A270" s="396"/>
-      <c r="B270" s="418"/>
-      <c r="C270" s="412"/>
+      <c r="A270" s="353"/>
+      <c r="B270" s="356"/>
+      <c r="C270" s="359"/>
       <c r="D270" s="284">
         <v>20</v>
       </c>
       <c r="E270" s="278"/>
     </row>
     <row r="271" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A271" s="396"/>
-      <c r="B271" s="419"/>
-      <c r="C271" s="413"/>
+      <c r="A271" s="353"/>
+      <c r="B271" s="357"/>
+      <c r="C271" s="360"/>
       <c r="D271" s="285">
         <v>21</v>
       </c>
       <c r="E271" s="279"/>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A272" s="396"/>
-      <c r="B272" s="417" t="s">
+      <c r="A272" s="353"/>
+      <c r="B272" s="355" t="s">
         <v>89</v>
       </c>
-      <c r="C272" s="411"/>
+      <c r="C272" s="358"/>
       <c r="D272" s="283">
         <v>22</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A273" s="396"/>
-      <c r="B273" s="418"/>
-      <c r="C273" s="412"/>
+      <c r="A273" s="353"/>
+      <c r="B273" s="356"/>
+      <c r="C273" s="359"/>
       <c r="D273" s="284">
         <v>23</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A274" s="396"/>
-      <c r="B274" s="418"/>
-      <c r="C274" s="412"/>
+      <c r="A274" s="353"/>
+      <c r="B274" s="356"/>
+      <c r="C274" s="359"/>
       <c r="D274" s="284">
         <v>24</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A275" s="396"/>
-      <c r="B275" s="418"/>
-      <c r="C275" s="412"/>
+      <c r="A275" s="353"/>
+      <c r="B275" s="356"/>
+      <c r="C275" s="359"/>
       <c r="D275" s="284">
         <v>25</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A276" s="396"/>
-      <c r="B276" s="418"/>
-      <c r="C276" s="412"/>
+      <c r="A276" s="353"/>
+      <c r="B276" s="356"/>
+      <c r="C276" s="359"/>
       <c r="D276" s="284">
         <v>26</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A277" s="396"/>
-      <c r="B277" s="418"/>
-      <c r="C277" s="412"/>
+      <c r="A277" s="353"/>
+      <c r="B277" s="356"/>
+      <c r="C277" s="359"/>
       <c r="D277" s="284">
         <v>27</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A278" s="396"/>
-      <c r="B278" s="419"/>
-      <c r="C278" s="413"/>
+      <c r="A278" s="353"/>
+      <c r="B278" s="357"/>
+      <c r="C278" s="360"/>
       <c r="D278" s="285">
         <v>28</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A279" s="396"/>
-      <c r="B279" s="417" t="s">
+      <c r="A279" s="353"/>
+      <c r="B279" s="355" t="s">
         <v>67</v>
       </c>
-      <c r="C279" s="411"/>
+      <c r="C279" s="358"/>
       <c r="D279" s="283">
         <v>29</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A280" s="396"/>
-      <c r="B280" s="418"/>
-      <c r="C280" s="412"/>
+      <c r="A280" s="353"/>
+      <c r="B280" s="356"/>
+      <c r="C280" s="359"/>
       <c r="D280" s="284">
         <v>30</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A281" s="396"/>
-      <c r="B281" s="418"/>
-      <c r="C281" s="412"/>
+      <c r="A281" s="353"/>
+      <c r="B281" s="356"/>
+      <c r="C281" s="359"/>
       <c r="D281" s="284">
         <v>31</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A282" s="396"/>
-      <c r="B282" s="418"/>
-      <c r="C282" s="412"/>
+      <c r="A282" s="353"/>
+      <c r="B282" s="356"/>
+      <c r="C282" s="359"/>
       <c r="D282" s="286"/>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A283" s="396"/>
-      <c r="B283" s="418"/>
-      <c r="C283" s="412"/>
+      <c r="A283" s="353"/>
+      <c r="B283" s="356"/>
+      <c r="C283" s="359"/>
       <c r="D283" s="286"/>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A284" s="396"/>
-      <c r="B284" s="418"/>
-      <c r="C284" s="412"/>
+      <c r="A284" s="353"/>
+      <c r="B284" s="356"/>
+      <c r="C284" s="359"/>
       <c r="D284" s="286"/>
     </row>
     <row r="285" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A285" s="394"/>
-      <c r="B285" s="419"/>
-      <c r="C285" s="413"/>
+      <c r="A285" s="354"/>
+      <c r="B285" s="357"/>
+      <c r="C285" s="360"/>
       <c r="D285" s="287"/>
     </row>
   </sheetData>
   <mergeCells count="198">
-    <mergeCell ref="A251:A285"/>
-    <mergeCell ref="B251:B257"/>
-    <mergeCell ref="C251:C257"/>
-    <mergeCell ref="B258:B264"/>
-    <mergeCell ref="C258:C264"/>
-    <mergeCell ref="B265:B271"/>
-    <mergeCell ref="C265:C271"/>
-    <mergeCell ref="B272:B278"/>
-    <mergeCell ref="C272:C278"/>
-    <mergeCell ref="B279:B285"/>
-    <mergeCell ref="C279:C285"/>
-    <mergeCell ref="A215:A249"/>
-    <mergeCell ref="B215:B221"/>
-    <mergeCell ref="C215:C221"/>
-    <mergeCell ref="B222:B228"/>
-    <mergeCell ref="C222:C228"/>
-    <mergeCell ref="B229:B235"/>
-    <mergeCell ref="C229:C235"/>
-    <mergeCell ref="B236:B242"/>
-    <mergeCell ref="C236:C242"/>
-    <mergeCell ref="B243:B249"/>
-    <mergeCell ref="C243:C249"/>
-    <mergeCell ref="G12:G18"/>
-    <mergeCell ref="G19:G25"/>
-    <mergeCell ref="G26:G32"/>
-    <mergeCell ref="G33:G39"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="B64:B73"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="B114:B123"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="B104:B113"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="B94:B103"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G169:G170"/>
+    <mergeCell ref="J169:J170"/>
+    <mergeCell ref="G171:G172"/>
+    <mergeCell ref="F173:F182"/>
+    <mergeCell ref="G173:G174"/>
+    <mergeCell ref="J173:J174"/>
+    <mergeCell ref="G175:G176"/>
+    <mergeCell ref="J175:J176"/>
+    <mergeCell ref="G177:G178"/>
+    <mergeCell ref="J177:J178"/>
+    <mergeCell ref="G179:G180"/>
+    <mergeCell ref="J179:J180"/>
+    <mergeCell ref="G181:G182"/>
+    <mergeCell ref="J181:J182"/>
+    <mergeCell ref="J171:J172"/>
+    <mergeCell ref="F163:F172"/>
+    <mergeCell ref="G163:G164"/>
+    <mergeCell ref="J163:J164"/>
+    <mergeCell ref="G167:G168"/>
+    <mergeCell ref="J167:J168"/>
+    <mergeCell ref="G159:G160"/>
+    <mergeCell ref="J159:J160"/>
+    <mergeCell ref="G141:G142"/>
+    <mergeCell ref="J141:J142"/>
+    <mergeCell ref="G143:G144"/>
+    <mergeCell ref="J143:J144"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="J145:J146"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="J147:J148"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="J149:J150"/>
+    <mergeCell ref="G151:G152"/>
+    <mergeCell ref="J151:J152"/>
+    <mergeCell ref="G153:G154"/>
+    <mergeCell ref="J153:J154"/>
+    <mergeCell ref="G155:G156"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="J155:J156"/>
+    <mergeCell ref="G157:G158"/>
+    <mergeCell ref="J157:J158"/>
+    <mergeCell ref="B74:B83"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="B84:B93"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="G165:G166"/>
     <mergeCell ref="J165:J166"/>
@@ -16899,144 +16999,42 @@
     <mergeCell ref="G5:G11"/>
     <mergeCell ref="G161:G162"/>
     <mergeCell ref="J161:J162"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="J155:J156"/>
-    <mergeCell ref="G157:G158"/>
-    <mergeCell ref="J157:J158"/>
-    <mergeCell ref="B74:B83"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="B84:B93"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="G159:G160"/>
-    <mergeCell ref="J159:J160"/>
-    <mergeCell ref="G141:G142"/>
-    <mergeCell ref="J141:J142"/>
-    <mergeCell ref="G143:G144"/>
-    <mergeCell ref="J143:J144"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="J145:J146"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="J147:J148"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="J149:J150"/>
-    <mergeCell ref="G151:G152"/>
-    <mergeCell ref="J151:J152"/>
-    <mergeCell ref="G153:G154"/>
-    <mergeCell ref="J153:J154"/>
-    <mergeCell ref="G155:G156"/>
-    <mergeCell ref="G169:G170"/>
-    <mergeCell ref="J169:J170"/>
-    <mergeCell ref="G171:G172"/>
-    <mergeCell ref="F173:F182"/>
-    <mergeCell ref="G173:G174"/>
-    <mergeCell ref="J173:J174"/>
-    <mergeCell ref="G175:G176"/>
-    <mergeCell ref="J175:J176"/>
-    <mergeCell ref="G177:G178"/>
-    <mergeCell ref="J177:J178"/>
-    <mergeCell ref="G179:G180"/>
-    <mergeCell ref="J179:J180"/>
-    <mergeCell ref="G181:G182"/>
-    <mergeCell ref="J181:J182"/>
-    <mergeCell ref="J171:J172"/>
-    <mergeCell ref="F163:F172"/>
-    <mergeCell ref="G163:G164"/>
-    <mergeCell ref="J163:J164"/>
-    <mergeCell ref="G167:G168"/>
-    <mergeCell ref="J167:J168"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="B94:B103"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="B64:B73"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="B114:B123"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="B104:B113"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="G12:G18"/>
+    <mergeCell ref="G19:G25"/>
+    <mergeCell ref="G26:G32"/>
+    <mergeCell ref="G33:G39"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A215:A249"/>
+    <mergeCell ref="B215:B221"/>
+    <mergeCell ref="C215:C221"/>
+    <mergeCell ref="B222:B228"/>
+    <mergeCell ref="C222:C228"/>
+    <mergeCell ref="B229:B235"/>
+    <mergeCell ref="C229:C235"/>
+    <mergeCell ref="B236:B242"/>
+    <mergeCell ref="C236:C242"/>
+    <mergeCell ref="B243:B249"/>
+    <mergeCell ref="C243:C249"/>
+    <mergeCell ref="A251:A285"/>
+    <mergeCell ref="B251:B257"/>
+    <mergeCell ref="C251:C257"/>
+    <mergeCell ref="B258:B264"/>
+    <mergeCell ref="C258:C264"/>
+    <mergeCell ref="B265:B271"/>
+    <mergeCell ref="C265:C271"/>
+    <mergeCell ref="B272:B278"/>
+    <mergeCell ref="C272:C278"/>
+    <mergeCell ref="B279:B285"/>
+    <mergeCell ref="C279:C285"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C86" r:id="rId1" location="inheritance" xr:uid="{D2CBA3C8-CB7C-434F-8220-58DD8B46E3B2}"/>
@@ -17504,49 +17502,49 @@
   <sheetData>
     <row r="2" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="420" t="s">
+      <c r="C3" s="421" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="421"/>
-      <c r="E3" s="422"/>
+      <c r="D3" s="422"/>
+      <c r="E3" s="423"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="371" t="s">
+      <c r="C4" s="368" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="423"/>
-      <c r="E4" s="372"/>
+      <c r="D4" s="424"/>
+      <c r="E4" s="369"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C5" s="373" t="s">
+      <c r="C5" s="372" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="424"/>
-      <c r="E5" s="363"/>
+      <c r="D5" s="420"/>
+      <c r="E5" s="373"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="373" t="s">
+      <c r="C6" s="372" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="424"/>
-      <c r="E6" s="363"/>
+      <c r="D6" s="420"/>
+      <c r="E6" s="373"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="373" t="s">
+      <c r="C7" s="372" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="424"/>
-      <c r="E7" s="363"/>
+      <c r="D7" s="420"/>
+      <c r="E7" s="373"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C8" s="373"/>
-      <c r="D8" s="424"/>
-      <c r="E8" s="363"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="420"/>
+      <c r="E8" s="373"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C9" s="373"/>
-      <c r="D9" s="424"/>
-      <c r="E9" s="363"/>
+      <c r="C9" s="372"/>
+      <c r="D9" s="420"/>
+      <c r="E9" s="373"/>
       <c r="I9" s="137"/>
       <c r="J9" s="137"/>
       <c r="K9" s="137"/>
@@ -17554,9 +17552,9 @@
       <c r="M9" s="137"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C10" s="373"/>
-      <c r="D10" s="424"/>
-      <c r="E10" s="363"/>
+      <c r="C10" s="372"/>
+      <c r="D10" s="420"/>
+      <c r="E10" s="373"/>
       <c r="H10" t="s">
         <v>35</v>
       </c>
@@ -17567,9 +17565,9 @@
       <c r="M10" s="137"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="373"/>
-      <c r="D11" s="424"/>
-      <c r="E11" s="363"/>
+      <c r="C11" s="372"/>
+      <c r="D11" s="420"/>
+      <c r="E11" s="373"/>
       <c r="I11" s="151"/>
       <c r="J11" s="151"/>
       <c r="K11" s="151"/>
@@ -17577,9 +17575,9 @@
       <c r="M11" s="137"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C12" s="373"/>
-      <c r="D12" s="424"/>
-      <c r="E12" s="363"/>
+      <c r="C12" s="372"/>
+      <c r="D12" s="420"/>
+      <c r="E12" s="373"/>
       <c r="I12" s="151"/>
       <c r="J12" s="151"/>
       <c r="K12" s="151"/>
@@ -17587,9 +17585,9 @@
       <c r="M12" s="137"/>
     </row>
     <row r="13" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="364"/>
-      <c r="D13" s="416"/>
-      <c r="E13" s="365"/>
+      <c r="C13" s="370"/>
+      <c r="D13" s="374"/>
+      <c r="E13" s="371"/>
       <c r="I13" s="151"/>
       <c r="J13" s="151"/>
       <c r="K13" s="151"/>
@@ -21449,17 +21447,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31" r:id="rId1" xr:uid="{1B01AA0E-43AB-4691-BAC5-AB91577CBAC7}"/>

</xml_diff>